<commit_message>
EPBDS-7754 Rename date() to Date()
Date() is more constructor-like and more friendly for understanding for BAs
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/Dates.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/Dates.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="toString" sheetId="8" r:id="rId1"/>
     <sheet name="toDate" sheetId="11" r:id="rId2"/>
-    <sheet name="date" sheetId="10" r:id="rId3"/>
+    <sheet name="Date" sheetId="10" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -297,9 +297,6 @@
     <t>07/07/7777777</t>
   </si>
   <si>
-    <t>return date(year, month, day);</t>
-  </si>
-  <si>
     <t>Test dateMethod</t>
   </si>
   <si>
@@ -313,6 +310,9 @@
   </si>
   <si>
     <t>Method Date dateMethod (int year, int month, int day)</t>
+  </si>
+  <si>
+    <t>return Date(year, month, day);</t>
   </si>
 </sst>
 </file>
@@ -542,6 +542,8 @@
     <xf numFmtId="166" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -557,8 +559,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -948,22 +948,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="24"/>
+      <c r="C2" s="26"/>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="C3" s="25"/>
+      <c r="C3" s="27"/>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="C5" s="23"/>
+      <c r="C5" s="25"/>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
@@ -1126,25 +1126,25 @@
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B29" s="24" t="s">
+      <c r="B29" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="C29" s="24"/>
-      <c r="D29" s="24"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B30" s="25" t="s">
+      <c r="B30" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="C30" s="25"/>
-      <c r="D30" s="25"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B32" s="21" t="s">
+      <c r="B32" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="C32" s="22"/>
-      <c r="D32" s="23"/>
+      <c r="C32" s="24"/>
+      <c r="D32" s="25"/>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B33" s="2" t="s">
@@ -1560,22 +1560,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="C2" s="24"/>
+      <c r="C2" s="26"/>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="C3" s="25"/>
+      <c r="C3" s="27"/>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="C5" s="23"/>
+      <c r="C5" s="25"/>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
@@ -1597,7 +1597,7 @@
       <c r="B8" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="26">
+      <c r="C8" s="21">
         <v>42124</v>
       </c>
     </row>
@@ -1605,7 +1605,7 @@
       <c r="B9" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="27" t="s">
+      <c r="C9" s="22" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1613,7 +1613,7 @@
       <c r="B10" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="C10" s="26">
+      <c r="C10" s="21">
         <v>40544</v>
       </c>
     </row>
@@ -1621,7 +1621,7 @@
       <c r="B11" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="27" t="s">
+      <c r="C11" s="22" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1629,7 +1629,7 @@
       <c r="B12" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="27" t="s">
+      <c r="C12" s="22" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1637,7 +1637,7 @@
       <c r="B13" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="27" t="s">
+      <c r="C13" s="22" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1645,7 +1645,7 @@
       <c r="B14" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="27" t="s">
+      <c r="C14" s="22" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1653,7 +1653,7 @@
       <c r="B15" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="27" t="s">
+      <c r="C15" s="22" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1661,7 +1661,7 @@
       <c r="B16" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="27" t="s">
+      <c r="C16" s="22" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1669,7 +1669,7 @@
       <c r="B17" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="27" t="s">
+      <c r="C17" s="22" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1677,7 +1677,7 @@
       <c r="B18" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="27" t="s">
+      <c r="C18" s="22" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1685,30 +1685,30 @@
       <c r="B19" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C19" s="27" t="s">
+      <c r="C19" s="22" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B23" s="24" t="s">
+      <c r="B23" s="26" t="s">
         <v>81</v>
       </c>
-      <c r="C23" s="24"/>
-      <c r="D23" s="24"/>
+      <c r="C23" s="26"/>
+      <c r="D23" s="26"/>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B24" s="25" t="s">
+      <c r="B24" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="C24" s="25"/>
-      <c r="D24" s="25"/>
+      <c r="C24" s="27"/>
+      <c r="D24" s="27"/>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B26" s="21" t="s">
+      <c r="B26" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="C26" s="22"/>
-      <c r="D26" s="23"/>
+      <c r="C26" s="24"/>
+      <c r="D26" s="25"/>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B27" s="2" t="s">
@@ -2096,12 +2096,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="B26:D26"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B23:D23"/>
     <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B26:D26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2113,7 +2113,7 @@
   <dimension ref="B4:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2123,22 +2123,22 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B5" s="27" t="s">
         <v>98</v>
       </c>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B5" s="25" t="s">
-        <v>93</v>
-      </c>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B7" s="28" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C7" s="29"/>
       <c r="D7" s="29"/>
@@ -2160,13 +2160,13 @@
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B9" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C9" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="D9" s="14" t="s">
         <v>96</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>97</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
EPBDS-7884 Return null instead of ParseException
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/Dates.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/Dates.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="0" windowWidth="16350" windowHeight="11760" tabRatio="833" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="0" windowWidth="16350" windowHeight="11760" tabRatio="833" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="toString" sheetId="8" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="107">
   <si>
     <t>_res_</t>
   </si>
@@ -313,6 +313,30 @@
   </si>
   <si>
     <t>return Date(year, month, day);</t>
+  </si>
+  <si>
+    <t>13/13/2018</t>
+  </si>
+  <si>
+    <t>as</t>
+  </si>
+  <si>
+    <t>_description_</t>
+  </si>
+  <si>
+    <t>null to null</t>
+  </si>
+  <si>
+    <t>wrong date</t>
+  </si>
+  <si>
+    <t>wrong format</t>
+  </si>
+  <si>
+    <t>12/12/2018</t>
+  </si>
+  <si>
+    <t>wrong input</t>
   </si>
 </sst>
 </file>
@@ -520,7 +544,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -568,6 +592,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1546,10 +1574,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D62"/>
+  <dimension ref="B2:E73"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23:D30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1559,33 +1587,36 @@
     <col min="4" max="5" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B2" s="26" t="s">
         <v>80</v>
       </c>
       <c r="C2" s="26"/>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B3" s="27" t="s">
         <v>73</v>
       </c>
       <c r="C3" s="27"/>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B5" s="23" t="s">
         <v>78</v>
       </c>
       <c r="C5" s="25"/>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
         <v>74</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="D6" s="34" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
         <v>75</v>
       </c>
@@ -1593,7 +1624,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B8" s="11" t="s">
         <v>10</v>
       </c>
@@ -1601,7 +1632,7 @@
         <v>42124</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B9" s="20" t="s">
         <v>9</v>
       </c>
@@ -1609,7 +1640,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B10" s="11" t="s">
         <v>76</v>
       </c>
@@ -1617,7 +1648,7 @@
         <v>40544</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B11" s="11" t="s">
         <v>6</v>
       </c>
@@ -1625,7 +1656,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B12" s="11" t="s">
         <v>7</v>
       </c>
@@ -1633,7 +1664,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B13" s="11" t="s">
         <v>8</v>
       </c>
@@ -1641,7 +1672,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B14" s="11" t="s">
         <v>5</v>
       </c>
@@ -1649,7 +1680,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B15" s="11" t="s">
         <v>31</v>
       </c>
@@ -1657,7 +1688,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B16" s="11" t="s">
         <v>32</v>
       </c>
@@ -1689,419 +1720,507 @@
         <v>39</v>
       </c>
     </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B20" s="22"/>
+      <c r="C20" s="22"/>
+      <c r="D20" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B21" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="C21" s="22"/>
+      <c r="D21" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B22" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="C22" s="22"/>
+      <c r="D22" t="s">
+        <v>106</v>
+      </c>
+    </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B23" s="26" t="s">
+      <c r="B23" s="31"/>
+      <c r="C23" s="32"/>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B24" s="31"/>
+      <c r="C24" s="32"/>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B25" s="31"/>
+      <c r="C25" s="32"/>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B26" s="31"/>
+      <c r="C26" s="32"/>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B30" s="26" t="s">
         <v>81</v>
       </c>
-      <c r="C23" s="26"/>
-      <c r="D23" s="26"/>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B24" s="27" t="s">
+      <c r="C30" s="26"/>
+      <c r="D30" s="26"/>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B31" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="C24" s="27"/>
-      <c r="D24" s="27"/>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B26" s="23" t="s">
+      <c r="C31" s="27"/>
+      <c r="D31" s="27"/>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B33" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="C26" s="24"/>
-      <c r="D26" s="25"/>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B27" s="2" t="s">
+      <c r="C33" s="24"/>
+      <c r="D33" s="25"/>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B34" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C27" s="13" t="s">
+      <c r="C34" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="D34" s="33" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B28" s="3" t="s">
+      <c r="E34" s="34" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B35" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C28" s="14" t="s">
+      <c r="C35" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="D35" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B29" s="11" t="s">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B36" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="C29" s="8" t="s">
+      <c r="C36" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="D29" s="11" t="s">
+      <c r="D36" s="11" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B30" s="11" t="s">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B37" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C30" s="8" t="s">
+      <c r="C37" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D30" s="11" t="s">
+      <c r="D37" s="11" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B31" s="11" t="s">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B38" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C31" s="8" t="s">
+      <c r="C38" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D31" s="11" t="s">
+      <c r="D38" s="11" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B32" s="11" t="s">
+    <row r="39" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B39" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C32" s="8" t="s">
+      <c r="C39" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D32" s="11" t="s">
+      <c r="D39" s="11" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B33" s="11" t="s">
+    <row r="40" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B40" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C33" s="8" t="s">
+      <c r="C40" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D33" s="11" t="s">
+      <c r="D40" s="11" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B34" s="11" t="s">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B41" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C34" s="8" t="s">
+      <c r="C41" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D34" s="11" t="s">
+      <c r="D41" s="11" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B35" s="11" t="s">
+    <row r="42" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B42" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C35" s="8" t="s">
+      <c r="C42" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D35" s="11" t="s">
+      <c r="D42" s="11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B36" s="11" t="s">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B43" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C36" s="5"/>
-      <c r="D36" s="11" t="s">
+      <c r="C43" s="5"/>
+      <c r="D43" s="11" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B37" s="11" t="s">
+    <row r="44" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B44" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C37" s="7"/>
-      <c r="D37" s="11" t="s">
+      <c r="C44" s="7"/>
+      <c r="D44" s="11" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B38" s="11" t="s">
+    <row r="45" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B45" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C38" s="10"/>
-      <c r="D38" s="11" t="s">
+      <c r="C45" s="10"/>
+      <c r="D45" s="11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B39" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="C39" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D39" s="11" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B40" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="C40" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D40" s="11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B41" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C41" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D41" s="9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B42" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C42" s="6"/>
-      <c r="D42" s="11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B43" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="C43" s="6"/>
-      <c r="D43" s="11" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B44" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C44" s="10"/>
-      <c r="D44" s="11" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B45" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="C45" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="D45" s="11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B46" s="9" t="s">
+    <row r="46" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B46" s="11" t="s">
         <v>36</v>
       </c>
       <c r="C46" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D46" s="9" t="s">
+      <c r="D46" s="11" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B47" s="11" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="C47" s="10" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="D47" s="11" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B48" s="9" t="s">
-        <v>39</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B48" s="11" t="s">
+        <v>24</v>
       </c>
       <c r="C48" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D48" s="11" t="s">
-        <v>39</v>
+      <c r="D48" s="9" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B49" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="C49" s="10" t="s">
-        <v>54</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="C49" s="6"/>
       <c r="D49" s="11" t="s">
-        <v>83</v>
+        <v>8</v>
       </c>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B50" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C50" s="10" t="s">
-        <v>13</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="C50" s="6"/>
       <c r="D50" s="11" t="s">
-        <v>3</v>
+        <v>55</v>
       </c>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B51" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="C51" s="10" t="s">
-        <v>48</v>
-      </c>
+      <c r="B51" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C51" s="10"/>
       <c r="D51" s="11" t="s">
-        <v>85</v>
+        <v>39</v>
       </c>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B52" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C52" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C52" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="D52" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B53" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C53" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D52" s="19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B53" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="C53" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="D53" s="11" t="s">
-        <v>86</v>
+      <c r="D53" s="9" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B54" s="11" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C54" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D54" s="11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B55" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C55" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D54" s="16" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B55" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="C55" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="D55" s="16" t="s">
-        <v>87</v>
+      <c r="D55" s="11" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B56" s="11" t="s">
-        <v>84</v>
+        <v>40</v>
       </c>
       <c r="C56" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D56" s="16" t="s">
-        <v>39</v>
+        <v>54</v>
+      </c>
+      <c r="D56" s="11" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B57" s="11" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="C57" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="D57" s="8">
-        <v>25599</v>
+        <v>13</v>
+      </c>
+      <c r="D57" s="11" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B58" s="11" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C58" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="D58" s="8">
-        <v>25903</v>
+        <v>48</v>
+      </c>
+      <c r="D58" s="11" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B59" s="11" t="s">
-        <v>88</v>
+        <v>8</v>
       </c>
       <c r="C59" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="D59" s="8">
-        <v>20090</v>
+        <v>13</v>
+      </c>
+      <c r="D59" s="19">
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B60" s="11" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="C60" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D60" s="8" t="s">
-        <v>7</v>
+        <v>50</v>
+      </c>
+      <c r="D60" s="11" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B61" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C61" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="D61" s="8" t="s">
-        <v>16</v>
+        <v>41</v>
+      </c>
+      <c r="C61" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D61" s="16" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B62" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C62" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D62" s="16" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="63" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B63" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="C63" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D63" s="16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="64" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B64" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C64" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D64" s="8">
+        <v>25599</v>
+      </c>
+    </row>
+    <row r="65" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B65" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C65" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D65" s="8">
+        <v>25903</v>
+      </c>
+    </row>
+    <row r="66" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B66" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="C66" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D66" s="8">
+        <v>20090</v>
+      </c>
+    </row>
+    <row r="67" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B67" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C67" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D67" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="68" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B68" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C68" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="D68" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="69" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B69" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C62" s="11" t="s">
+      <c r="C69" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="D62" s="11" t="s">
+      <c r="D69" s="11" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="70" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B70" s="10"/>
+      <c r="C70" s="10"/>
+      <c r="D70" s="10"/>
+      <c r="E70" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="71" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B71" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="C71" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D71" s="10"/>
+      <c r="E71" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="72" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B72" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="C72" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D72" s="10"/>
+      <c r="E72" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="73" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B73" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="C73" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="D73" s="10"/>
+      <c r="E73" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B33:D33"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B31:D31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2112,7 +2231,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
EPDBS-7884 Move isDate() to Dates
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/Dates.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/Dates.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="0" windowWidth="16350" windowHeight="11760" tabRatio="833" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="0" windowWidth="16350" windowHeight="11760" tabRatio="833" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="toString" sheetId="8" r:id="rId1"/>
     <sheet name="toDate" sheetId="11" r:id="rId2"/>
     <sheet name="Date" sheetId="10" r:id="rId3"/>
+    <sheet name="isDate" sheetId="12" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="139">
   <si>
     <t>_res_</t>
   </si>
@@ -337,6 +338,102 @@
   </si>
   <si>
     <t>wrong input</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>06/17/2014</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>MM.dd.yyyy</t>
+  </si>
+  <si>
+    <t>06/27.2014</t>
+  </si>
+  <si>
+    <t>06.27.2014</t>
+  </si>
+  <si>
+    <t>oo.oo.2014</t>
+  </si>
+  <si>
+    <t>31/17/2014</t>
+  </si>
+  <si>
+    <t>2014-12-12</t>
+  </si>
+  <si>
+    <t>yyyy-MM-dd</t>
+  </si>
+  <si>
+    <t>2014-13-12</t>
+  </si>
+  <si>
+    <t>123456789</t>
+  </si>
+  <si>
+    <t>12.30</t>
+  </si>
+  <si>
+    <t>yyy-dd-MM</t>
+  </si>
+  <si>
+    <t>foo</t>
+  </si>
+  <si>
+    <t>Empty</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Pattern</t>
+  </si>
+  <si>
+    <t>Test isDateMethod</t>
+  </si>
+  <si>
+    <t>Test isDateMethodWhenObject</t>
+  </si>
+  <si>
+    <t>Test isDateMethodWhenDate</t>
+  </si>
+  <si>
+    <t>Test isDateWithPatternMethod</t>
+  </si>
+  <si>
+    <t>return isDate(new Object());</t>
+  </si>
+  <si>
+    <t>return isDate(date);</t>
+  </si>
+  <si>
+    <t>return isDate(str, pattern);</t>
+  </si>
+  <si>
+    <t>return isDate(str);</t>
+  </si>
+  <si>
+    <t>Method boolean isDateMethodWhenObject()</t>
+  </si>
+  <si>
+    <t>Method boolean isDateMethodWhenDate(Date date)</t>
+  </si>
+  <si>
+    <t>Method boolean isDateWithPatternMethod(String str, String pattern)</t>
+  </si>
+  <si>
+    <t>Method boolean isDateMethod(String str)</t>
   </si>
 </sst>
 </file>
@@ -544,7 +641,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -568,6 +665,10 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -592,10 +693,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -976,22 +1079,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="26"/>
+      <c r="C2" s="30"/>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="C3" s="27"/>
+      <c r="C3" s="31"/>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="C5" s="25"/>
+      <c r="C5" s="29"/>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
@@ -1154,25 +1257,25 @@
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B29" s="26" t="s">
+      <c r="B29" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="C29" s="26"/>
-      <c r="D29" s="26"/>
+      <c r="C29" s="30"/>
+      <c r="D29" s="30"/>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B30" s="27" t="s">
+      <c r="B30" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="31"/>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B32" s="23" t="s">
+      <c r="B32" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="C32" s="24"/>
-      <c r="D32" s="25"/>
+      <c r="C32" s="28"/>
+      <c r="D32" s="29"/>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B33" s="2" t="s">
@@ -1576,7 +1679,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
@@ -1588,22 +1691,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="C2" s="26"/>
+      <c r="C2" s="30"/>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="C3" s="27"/>
+      <c r="C3" s="31"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="C5" s="25"/>
+      <c r="C5" s="29"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
@@ -1612,7 +1715,7 @@
       <c r="C6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="34" t="s">
+      <c r="D6" s="26" t="s">
         <v>101</v>
       </c>
     </row>
@@ -1746,41 +1849,41 @@
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B23" s="31"/>
-      <c r="C23" s="32"/>
+      <c r="B23" s="23"/>
+      <c r="C23" s="24"/>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B24" s="31"/>
-      <c r="C24" s="32"/>
+      <c r="B24" s="23"/>
+      <c r="C24" s="24"/>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B25" s="31"/>
-      <c r="C25" s="32"/>
+      <c r="B25" s="23"/>
+      <c r="C25" s="24"/>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B26" s="31"/>
-      <c r="C26" s="32"/>
+      <c r="B26" s="23"/>
+      <c r="C26" s="24"/>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B30" s="26" t="s">
+      <c r="B30" s="30" t="s">
         <v>81</v>
       </c>
-      <c r="C30" s="26"/>
-      <c r="D30" s="26"/>
+      <c r="C30" s="30"/>
+      <c r="D30" s="30"/>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B31" s="27" t="s">
+      <c r="B31" s="31" t="s">
         <v>77</v>
       </c>
-      <c r="C31" s="27"/>
-      <c r="D31" s="27"/>
+      <c r="C31" s="31"/>
+      <c r="D31" s="31"/>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B33" s="23" t="s">
+      <c r="B33" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="C33" s="24"/>
-      <c r="D33" s="25"/>
+      <c r="C33" s="28"/>
+      <c r="D33" s="29"/>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B34" s="2" t="s">
@@ -1789,10 +1892,10 @@
       <c r="C34" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="D34" s="33" t="s">
+      <c r="D34" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="E34" s="34" t="s">
+      <c r="E34" s="26" t="s">
         <v>101</v>
       </c>
     </row>
@@ -2242,26 +2345,26 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="30" t="s">
         <v>97</v>
       </c>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="31" t="s">
         <v>98</v>
       </c>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B7" s="28" t="s">
+      <c r="B7" s="32" t="s">
         <v>93</v>
       </c>
-      <c r="C7" s="29"/>
-      <c r="D7" s="29"/>
-      <c r="E7" s="30"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="34"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
@@ -2369,4 +2472,420 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:Y38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" customWidth="1"/>
+    <col min="16" max="16" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B2" s="37" t="s">
+        <v>138</v>
+      </c>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="G2" s="37" t="s">
+        <v>137</v>
+      </c>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="37"/>
+      <c r="O2" s="37" t="s">
+        <v>136</v>
+      </c>
+      <c r="P2" s="37"/>
+      <c r="Q2" s="37"/>
+      <c r="R2" s="37"/>
+      <c r="S2" s="37"/>
+      <c r="U2" s="37" t="s">
+        <v>135</v>
+      </c>
+      <c r="V2" s="37"/>
+      <c r="W2" s="37"/>
+      <c r="X2" s="37"/>
+      <c r="Y2" s="37"/>
+    </row>
+    <row r="3" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B3" s="37" t="s">
+        <v>134</v>
+      </c>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="G3" s="37" t="s">
+        <v>133</v>
+      </c>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
+      <c r="K3" s="37"/>
+      <c r="L3" s="37"/>
+      <c r="M3" s="37"/>
+      <c r="O3" s="37" t="s">
+        <v>132</v>
+      </c>
+      <c r="P3" s="37"/>
+      <c r="Q3" s="37"/>
+      <c r="R3" s="37"/>
+      <c r="S3" s="37"/>
+      <c r="U3" s="37" t="s">
+        <v>131</v>
+      </c>
+      <c r="V3" s="37"/>
+      <c r="W3" s="37"/>
+      <c r="X3" s="37"/>
+      <c r="Y3" s="37"/>
+    </row>
+    <row r="6" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="G6" s="37" t="s">
+        <v>130</v>
+      </c>
+      <c r="H6" s="37"/>
+      <c r="I6" s="37"/>
+      <c r="J6" s="37"/>
+      <c r="O6" s="37" t="s">
+        <v>129</v>
+      </c>
+      <c r="P6" s="37"/>
+      <c r="Q6" s="37"/>
+      <c r="R6" s="38"/>
+      <c r="U6" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="7" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B7" s="37" t="s">
+        <v>127</v>
+      </c>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="G7" t="s">
+        <v>101</v>
+      </c>
+      <c r="H7" t="s">
+        <v>74</v>
+      </c>
+      <c r="I7" t="s">
+        <v>65</v>
+      </c>
+      <c r="J7" t="s">
+        <v>0</v>
+      </c>
+      <c r="O7" t="s">
+        <v>101</v>
+      </c>
+      <c r="P7" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>0</v>
+      </c>
+      <c r="U7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>101</v>
+      </c>
+      <c r="C8" t="s">
+        <v>74</v>
+      </c>
+      <c r="D8" t="s">
+        <v>0</v>
+      </c>
+      <c r="G8" t="s">
+        <v>124</v>
+      </c>
+      <c r="H8" t="s">
+        <v>123</v>
+      </c>
+      <c r="I8" t="s">
+        <v>126</v>
+      </c>
+      <c r="J8" t="s">
+        <v>1</v>
+      </c>
+      <c r="O8" t="s">
+        <v>124</v>
+      </c>
+      <c r="P8" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>1</v>
+      </c>
+      <c r="U8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>124</v>
+      </c>
+      <c r="C9" t="s">
+        <v>123</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1</v>
+      </c>
+      <c r="G9" t="s">
+        <v>122</v>
+      </c>
+      <c r="H9" s="35"/>
+      <c r="J9" t="s">
+        <v>109</v>
+      </c>
+      <c r="O9" t="s">
+        <v>122</v>
+      </c>
+      <c r="P9" s="35"/>
+      <c r="Q9" t="s">
+        <v>109</v>
+      </c>
+      <c r="U9" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="10" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>122</v>
+      </c>
+      <c r="D10" t="s">
+        <v>109</v>
+      </c>
+      <c r="H10" s="35" t="s">
+        <v>108</v>
+      </c>
+      <c r="J10" t="s">
+        <v>107</v>
+      </c>
+      <c r="P10" s="36">
+        <v>41255</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="11" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="C11" s="35" t="s">
+        <v>121</v>
+      </c>
+      <c r="D11" t="s">
+        <v>109</v>
+      </c>
+      <c r="H11" s="35"/>
+      <c r="I11" t="s">
+        <v>120</v>
+      </c>
+      <c r="J11" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="C12" s="35" t="s">
+        <v>119</v>
+      </c>
+      <c r="D12" t="s">
+        <v>109</v>
+      </c>
+      <c r="H12" s="35" t="s">
+        <v>115</v>
+      </c>
+      <c r="I12" t="s">
+        <v>116</v>
+      </c>
+      <c r="J12" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="13" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="C13" s="35" t="s">
+        <v>118</v>
+      </c>
+      <c r="D13" t="s">
+        <v>109</v>
+      </c>
+      <c r="H13" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="I13" t="s">
+        <v>116</v>
+      </c>
+      <c r="J13" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="14" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="C14" s="35" t="s">
+        <v>115</v>
+      </c>
+      <c r="D14" t="s">
+        <v>109</v>
+      </c>
+      <c r="H14" s="35" t="s">
+        <v>112</v>
+      </c>
+      <c r="I14" t="s">
+        <v>110</v>
+      </c>
+      <c r="J14" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="15" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="C15" s="35" t="s">
+        <v>114</v>
+      </c>
+      <c r="D15" t="s">
+        <v>109</v>
+      </c>
+      <c r="H15" s="35" t="s">
+        <v>113</v>
+      </c>
+      <c r="I15" t="s">
+        <v>110</v>
+      </c>
+      <c r="J15" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="16" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="C16" s="35" t="s">
+        <v>112</v>
+      </c>
+      <c r="D16" t="s">
+        <v>109</v>
+      </c>
+      <c r="H16" s="35" t="s">
+        <v>111</v>
+      </c>
+      <c r="I16" t="s">
+        <v>110</v>
+      </c>
+      <c r="J16" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="17" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C17" s="35" t="s">
+        <v>108</v>
+      </c>
+      <c r="D17" t="s">
+        <v>107</v>
+      </c>
+      <c r="H17" s="35"/>
+    </row>
+    <row r="18" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="H18" s="35"/>
+    </row>
+    <row r="19" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="H19" s="35"/>
+    </row>
+    <row r="20" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C20" s="35"/>
+      <c r="H20" s="35"/>
+    </row>
+    <row r="21" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C21" s="35"/>
+      <c r="H21" s="35"/>
+    </row>
+    <row r="22" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C22" s="35"/>
+      <c r="H22" s="35"/>
+    </row>
+    <row r="23" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C23" s="35"/>
+      <c r="H23" s="35"/>
+    </row>
+    <row r="24" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C24" s="35"/>
+      <c r="H24" s="35"/>
+    </row>
+    <row r="25" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C25" s="35"/>
+      <c r="H25" s="35"/>
+    </row>
+    <row r="26" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C26" s="35"/>
+      <c r="H26" s="35"/>
+    </row>
+    <row r="27" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C27" s="35"/>
+      <c r="H27" s="35"/>
+    </row>
+    <row r="28" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C28" s="35"/>
+      <c r="H28" s="35"/>
+    </row>
+    <row r="29" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C29" s="35"/>
+      <c r="H29" s="35"/>
+    </row>
+    <row r="30" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C30" s="35"/>
+      <c r="H30" s="35"/>
+    </row>
+    <row r="31" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C31" s="35"/>
+      <c r="H31" s="35"/>
+    </row>
+    <row r="32" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C32" s="35"/>
+      <c r="H32" s="35"/>
+    </row>
+    <row r="33" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C33" s="35"/>
+      <c r="H33" s="35"/>
+    </row>
+    <row r="34" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C34" s="35"/>
+      <c r="H34" s="35"/>
+    </row>
+    <row r="35" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="H35" s="35"/>
+    </row>
+    <row r="36" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="H36" s="35"/>
+    </row>
+    <row r="37" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="H37" s="35"/>
+    </row>
+    <row r="38" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="H38" s="35"/>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="G3:M3"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="U2:Y2"/>
+    <mergeCell ref="U3:Y3"/>
+    <mergeCell ref="O2:S2"/>
+    <mergeCell ref="O3:S3"/>
+    <mergeCell ref="G6:J6"/>
+    <mergeCell ref="O6:Q6"/>
+    <mergeCell ref="G2:M2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
EPBDS-7884 Backed out changeset: fde1b1305896 Redudant functions
After discussing with BAs, they wanted to have such functions to prevent runtime errors.
Because of toXXX functions are tolerante to input errors, it does not need to check these inputs.
So it was decided to remove isXXX functions. Anyway if somebody will want to check format,
it is possible to achieve it using like() or isEmpty(toXXX()) functions.

--HG--
branch : 5.21.x
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/Dates.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/Dates.xlsx
@@ -4,20 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="0" windowWidth="16350" windowHeight="11760" tabRatio="833" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="0" windowWidth="16350" windowHeight="11760" tabRatio="833" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="toString" sheetId="8" r:id="rId1"/>
     <sheet name="toDate" sheetId="11" r:id="rId2"/>
     <sheet name="Date" sheetId="10" r:id="rId3"/>
-    <sheet name="isDate" sheetId="12" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="107">
   <si>
     <t>_res_</t>
   </si>
@@ -338,102 +337,6 @@
   </si>
   <si>
     <t>wrong input</t>
-  </si>
-  <si>
-    <t>true</t>
-  </si>
-  <si>
-    <t>06/17/2014</t>
-  </si>
-  <si>
-    <t>false</t>
-  </si>
-  <si>
-    <t>MM.dd.yyyy</t>
-  </si>
-  <si>
-    <t>06/27.2014</t>
-  </si>
-  <si>
-    <t>06.27.2014</t>
-  </si>
-  <si>
-    <t>oo.oo.2014</t>
-  </si>
-  <si>
-    <t>31/17/2014</t>
-  </si>
-  <si>
-    <t>2014-12-12</t>
-  </si>
-  <si>
-    <t>yyyy-MM-dd</t>
-  </si>
-  <si>
-    <t>2014-13-12</t>
-  </si>
-  <si>
-    <t>123456789</t>
-  </si>
-  <si>
-    <t>12.30</t>
-  </si>
-  <si>
-    <t>yyy-dd-MM</t>
-  </si>
-  <si>
-    <t>foo</t>
-  </si>
-  <si>
-    <t>Empty</t>
-  </si>
-  <si>
-    <t>String</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Pattern</t>
-  </si>
-  <si>
-    <t>Test isDateMethod</t>
-  </si>
-  <si>
-    <t>Test isDateMethodWhenObject</t>
-  </si>
-  <si>
-    <t>Test isDateMethodWhenDate</t>
-  </si>
-  <si>
-    <t>Test isDateWithPatternMethod</t>
-  </si>
-  <si>
-    <t>return isDate(new Object());</t>
-  </si>
-  <si>
-    <t>return isDate(date);</t>
-  </si>
-  <si>
-    <t>return isDate(str, pattern);</t>
-  </si>
-  <si>
-    <t>return isDate(str);</t>
-  </si>
-  <si>
-    <t>Method boolean isDateMethodWhenObject()</t>
-  </si>
-  <si>
-    <t>Method boolean isDateMethodWhenDate(Date date)</t>
-  </si>
-  <si>
-    <t>Method boolean isDateWithPatternMethod(String str, String pattern)</t>
-  </si>
-  <si>
-    <t>Method boolean isDateMethod(String str)</t>
   </si>
 </sst>
 </file>
@@ -641,7 +544,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -693,12 +596,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1679,8 +1576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E73"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C2"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="C96" sqref="C96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2334,7 +2231,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
@@ -2472,420 +2369,4 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:Y38"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" customWidth="1"/>
-    <col min="9" max="9" width="11.85546875" customWidth="1"/>
-    <col min="16" max="16" width="10.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B2" s="37" t="s">
-        <v>138</v>
-      </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="G2" s="37" t="s">
-        <v>137</v>
-      </c>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37"/>
-      <c r="O2" s="37" t="s">
-        <v>136</v>
-      </c>
-      <c r="P2" s="37"/>
-      <c r="Q2" s="37"/>
-      <c r="R2" s="37"/>
-      <c r="S2" s="37"/>
-      <c r="U2" s="37" t="s">
-        <v>135</v>
-      </c>
-      <c r="V2" s="37"/>
-      <c r="W2" s="37"/>
-      <c r="X2" s="37"/>
-      <c r="Y2" s="37"/>
-    </row>
-    <row r="3" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B3" s="37" t="s">
-        <v>134</v>
-      </c>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="G3" s="37" t="s">
-        <v>133</v>
-      </c>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
-      <c r="K3" s="37"/>
-      <c r="L3" s="37"/>
-      <c r="M3" s="37"/>
-      <c r="O3" s="37" t="s">
-        <v>132</v>
-      </c>
-      <c r="P3" s="37"/>
-      <c r="Q3" s="37"/>
-      <c r="R3" s="37"/>
-      <c r="S3" s="37"/>
-      <c r="U3" s="37" t="s">
-        <v>131</v>
-      </c>
-      <c r="V3" s="37"/>
-      <c r="W3" s="37"/>
-      <c r="X3" s="37"/>
-      <c r="Y3" s="37"/>
-    </row>
-    <row r="6" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="G6" s="37" t="s">
-        <v>130</v>
-      </c>
-      <c r="H6" s="37"/>
-      <c r="I6" s="37"/>
-      <c r="J6" s="37"/>
-      <c r="O6" s="37" t="s">
-        <v>129</v>
-      </c>
-      <c r="P6" s="37"/>
-      <c r="Q6" s="37"/>
-      <c r="R6" s="38"/>
-      <c r="U6" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="7" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B7" s="37" t="s">
-        <v>127</v>
-      </c>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37"/>
-      <c r="G7" t="s">
-        <v>101</v>
-      </c>
-      <c r="H7" t="s">
-        <v>74</v>
-      </c>
-      <c r="I7" t="s">
-        <v>65</v>
-      </c>
-      <c r="J7" t="s">
-        <v>0</v>
-      </c>
-      <c r="O7" t="s">
-        <v>101</v>
-      </c>
-      <c r="P7" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>0</v>
-      </c>
-      <c r="U7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B8" t="s">
-        <v>101</v>
-      </c>
-      <c r="C8" t="s">
-        <v>74</v>
-      </c>
-      <c r="D8" t="s">
-        <v>0</v>
-      </c>
-      <c r="G8" t="s">
-        <v>124</v>
-      </c>
-      <c r="H8" t="s">
-        <v>123</v>
-      </c>
-      <c r="I8" t="s">
-        <v>126</v>
-      </c>
-      <c r="J8" t="s">
-        <v>1</v>
-      </c>
-      <c r="O8" t="s">
-        <v>124</v>
-      </c>
-      <c r="P8" t="s">
-        <v>125</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>1</v>
-      </c>
-      <c r="U8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B9" t="s">
-        <v>124</v>
-      </c>
-      <c r="C9" t="s">
-        <v>123</v>
-      </c>
-      <c r="D9" t="s">
-        <v>1</v>
-      </c>
-      <c r="G9" t="s">
-        <v>122</v>
-      </c>
-      <c r="H9" s="35"/>
-      <c r="J9" t="s">
-        <v>109</v>
-      </c>
-      <c r="O9" t="s">
-        <v>122</v>
-      </c>
-      <c r="P9" s="35"/>
-      <c r="Q9" t="s">
-        <v>109</v>
-      </c>
-      <c r="U9" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="10" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B10" t="s">
-        <v>122</v>
-      </c>
-      <c r="D10" t="s">
-        <v>109</v>
-      </c>
-      <c r="H10" s="35" t="s">
-        <v>108</v>
-      </c>
-      <c r="J10" t="s">
-        <v>107</v>
-      </c>
-      <c r="P10" s="36">
-        <v>41255</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="11" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="C11" s="35" t="s">
-        <v>121</v>
-      </c>
-      <c r="D11" t="s">
-        <v>109</v>
-      </c>
-      <c r="H11" s="35"/>
-      <c r="I11" t="s">
-        <v>120</v>
-      </c>
-      <c r="J11" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="12" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="C12" s="35" t="s">
-        <v>119</v>
-      </c>
-      <c r="D12" t="s">
-        <v>109</v>
-      </c>
-      <c r="H12" s="35" t="s">
-        <v>115</v>
-      </c>
-      <c r="I12" t="s">
-        <v>116</v>
-      </c>
-      <c r="J12" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="13" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="C13" s="35" t="s">
-        <v>118</v>
-      </c>
-      <c r="D13" t="s">
-        <v>109</v>
-      </c>
-      <c r="H13" s="35" t="s">
-        <v>117</v>
-      </c>
-      <c r="I13" t="s">
-        <v>116</v>
-      </c>
-      <c r="J13" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="14" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="C14" s="35" t="s">
-        <v>115</v>
-      </c>
-      <c r="D14" t="s">
-        <v>109</v>
-      </c>
-      <c r="H14" s="35" t="s">
-        <v>112</v>
-      </c>
-      <c r="I14" t="s">
-        <v>110</v>
-      </c>
-      <c r="J14" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="15" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="C15" s="35" t="s">
-        <v>114</v>
-      </c>
-      <c r="D15" t="s">
-        <v>109</v>
-      </c>
-      <c r="H15" s="35" t="s">
-        <v>113</v>
-      </c>
-      <c r="I15" t="s">
-        <v>110</v>
-      </c>
-      <c r="J15" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="16" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="C16" s="35" t="s">
-        <v>112</v>
-      </c>
-      <c r="D16" t="s">
-        <v>109</v>
-      </c>
-      <c r="H16" s="35" t="s">
-        <v>111</v>
-      </c>
-      <c r="I16" t="s">
-        <v>110</v>
-      </c>
-      <c r="J16" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="17" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C17" s="35" t="s">
-        <v>108</v>
-      </c>
-      <c r="D17" t="s">
-        <v>107</v>
-      </c>
-      <c r="H17" s="35"/>
-    </row>
-    <row r="18" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="H18" s="35"/>
-    </row>
-    <row r="19" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="H19" s="35"/>
-    </row>
-    <row r="20" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C20" s="35"/>
-      <c r="H20" s="35"/>
-    </row>
-    <row r="21" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C21" s="35"/>
-      <c r="H21" s="35"/>
-    </row>
-    <row r="22" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C22" s="35"/>
-      <c r="H22" s="35"/>
-    </row>
-    <row r="23" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C23" s="35"/>
-      <c r="H23" s="35"/>
-    </row>
-    <row r="24" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C24" s="35"/>
-      <c r="H24" s="35"/>
-    </row>
-    <row r="25" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C25" s="35"/>
-      <c r="H25" s="35"/>
-    </row>
-    <row r="26" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C26" s="35"/>
-      <c r="H26" s="35"/>
-    </row>
-    <row r="27" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C27" s="35"/>
-      <c r="H27" s="35"/>
-    </row>
-    <row r="28" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C28" s="35"/>
-      <c r="H28" s="35"/>
-    </row>
-    <row r="29" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C29" s="35"/>
-      <c r="H29" s="35"/>
-    </row>
-    <row r="30" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C30" s="35"/>
-      <c r="H30" s="35"/>
-    </row>
-    <row r="31" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C31" s="35"/>
-      <c r="H31" s="35"/>
-    </row>
-    <row r="32" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C32" s="35"/>
-      <c r="H32" s="35"/>
-    </row>
-    <row r="33" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C33" s="35"/>
-      <c r="H33" s="35"/>
-    </row>
-    <row r="34" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C34" s="35"/>
-      <c r="H34" s="35"/>
-    </row>
-    <row r="35" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="H35" s="35"/>
-    </row>
-    <row r="36" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="H36" s="35"/>
-    </row>
-    <row r="37" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="H37" s="35"/>
-    </row>
-    <row r="38" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="H38" s="35"/>
-    </row>
-  </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="G3:M3"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="U2:Y2"/>
-    <mergeCell ref="U3:Y3"/>
-    <mergeCell ref="O2:S2"/>
-    <mergeCell ref="O3:S3"/>
-    <mergeCell ref="G6:J6"/>
-    <mergeCell ref="O6:Q6"/>
-    <mergeCell ref="G2:M2"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
EPBDS-7884 Backed out changeset: fde1b1305896 Redundant functions
After discussing with BAs, they wanted to have such functions to prevent runtime errors.
Because of toXXX functions are tolerante to input errors, it does not need to check these inputs.
So it was decided to remove isXXX functions. Anyway if somebody will want to check format,
it is possible to achieve it using like() or isEmpty(toXXX()) functions.
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/Dates.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/Dates.xlsx
@@ -4,20 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="0" windowWidth="16350" windowHeight="11760" tabRatio="833" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="0" windowWidth="16350" windowHeight="11760" tabRatio="833" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="toString" sheetId="8" r:id="rId1"/>
     <sheet name="toDate" sheetId="11" r:id="rId2"/>
     <sheet name="Date" sheetId="10" r:id="rId3"/>
-    <sheet name="isDate" sheetId="12" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="107">
   <si>
     <t>_res_</t>
   </si>
@@ -338,102 +337,6 @@
   </si>
   <si>
     <t>wrong input</t>
-  </si>
-  <si>
-    <t>true</t>
-  </si>
-  <si>
-    <t>06/17/2014</t>
-  </si>
-  <si>
-    <t>false</t>
-  </si>
-  <si>
-    <t>MM.dd.yyyy</t>
-  </si>
-  <si>
-    <t>06/27.2014</t>
-  </si>
-  <si>
-    <t>06.27.2014</t>
-  </si>
-  <si>
-    <t>oo.oo.2014</t>
-  </si>
-  <si>
-    <t>31/17/2014</t>
-  </si>
-  <si>
-    <t>2014-12-12</t>
-  </si>
-  <si>
-    <t>yyyy-MM-dd</t>
-  </si>
-  <si>
-    <t>2014-13-12</t>
-  </si>
-  <si>
-    <t>123456789</t>
-  </si>
-  <si>
-    <t>12.30</t>
-  </si>
-  <si>
-    <t>yyy-dd-MM</t>
-  </si>
-  <si>
-    <t>foo</t>
-  </si>
-  <si>
-    <t>Empty</t>
-  </si>
-  <si>
-    <t>String</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Pattern</t>
-  </si>
-  <si>
-    <t>Test isDateMethod</t>
-  </si>
-  <si>
-    <t>Test isDateMethodWhenObject</t>
-  </si>
-  <si>
-    <t>Test isDateMethodWhenDate</t>
-  </si>
-  <si>
-    <t>Test isDateWithPatternMethod</t>
-  </si>
-  <si>
-    <t>return isDate(new Object());</t>
-  </si>
-  <si>
-    <t>return isDate(date);</t>
-  </si>
-  <si>
-    <t>return isDate(str, pattern);</t>
-  </si>
-  <si>
-    <t>return isDate(str);</t>
-  </si>
-  <si>
-    <t>Method boolean isDateMethodWhenObject()</t>
-  </si>
-  <si>
-    <t>Method boolean isDateMethodWhenDate(Date date)</t>
-  </si>
-  <si>
-    <t>Method boolean isDateWithPatternMethod(String str, String pattern)</t>
-  </si>
-  <si>
-    <t>Method boolean isDateMethod(String str)</t>
   </si>
 </sst>
 </file>
@@ -641,7 +544,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -693,12 +596,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1679,8 +1576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E73"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C2"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="C96" sqref="C96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2334,7 +2231,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
@@ -2472,420 +2369,4 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:Y38"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" customWidth="1"/>
-    <col min="9" max="9" width="11.85546875" customWidth="1"/>
-    <col min="16" max="16" width="10.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B2" s="37" t="s">
-        <v>138</v>
-      </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="G2" s="37" t="s">
-        <v>137</v>
-      </c>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37"/>
-      <c r="O2" s="37" t="s">
-        <v>136</v>
-      </c>
-      <c r="P2" s="37"/>
-      <c r="Q2" s="37"/>
-      <c r="R2" s="37"/>
-      <c r="S2" s="37"/>
-      <c r="U2" s="37" t="s">
-        <v>135</v>
-      </c>
-      <c r="V2" s="37"/>
-      <c r="W2" s="37"/>
-      <c r="X2" s="37"/>
-      <c r="Y2" s="37"/>
-    </row>
-    <row r="3" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B3" s="37" t="s">
-        <v>134</v>
-      </c>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="G3" s="37" t="s">
-        <v>133</v>
-      </c>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
-      <c r="K3" s="37"/>
-      <c r="L3" s="37"/>
-      <c r="M3" s="37"/>
-      <c r="O3" s="37" t="s">
-        <v>132</v>
-      </c>
-      <c r="P3" s="37"/>
-      <c r="Q3" s="37"/>
-      <c r="R3" s="37"/>
-      <c r="S3" s="37"/>
-      <c r="U3" s="37" t="s">
-        <v>131</v>
-      </c>
-      <c r="V3" s="37"/>
-      <c r="W3" s="37"/>
-      <c r="X3" s="37"/>
-      <c r="Y3" s="37"/>
-    </row>
-    <row r="6" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="G6" s="37" t="s">
-        <v>130</v>
-      </c>
-      <c r="H6" s="37"/>
-      <c r="I6" s="37"/>
-      <c r="J6" s="37"/>
-      <c r="O6" s="37" t="s">
-        <v>129</v>
-      </c>
-      <c r="P6" s="37"/>
-      <c r="Q6" s="37"/>
-      <c r="R6" s="38"/>
-      <c r="U6" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="7" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B7" s="37" t="s">
-        <v>127</v>
-      </c>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37"/>
-      <c r="G7" t="s">
-        <v>101</v>
-      </c>
-      <c r="H7" t="s">
-        <v>74</v>
-      </c>
-      <c r="I7" t="s">
-        <v>65</v>
-      </c>
-      <c r="J7" t="s">
-        <v>0</v>
-      </c>
-      <c r="O7" t="s">
-        <v>101</v>
-      </c>
-      <c r="P7" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>0</v>
-      </c>
-      <c r="U7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B8" t="s">
-        <v>101</v>
-      </c>
-      <c r="C8" t="s">
-        <v>74</v>
-      </c>
-      <c r="D8" t="s">
-        <v>0</v>
-      </c>
-      <c r="G8" t="s">
-        <v>124</v>
-      </c>
-      <c r="H8" t="s">
-        <v>123</v>
-      </c>
-      <c r="I8" t="s">
-        <v>126</v>
-      </c>
-      <c r="J8" t="s">
-        <v>1</v>
-      </c>
-      <c r="O8" t="s">
-        <v>124</v>
-      </c>
-      <c r="P8" t="s">
-        <v>125</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>1</v>
-      </c>
-      <c r="U8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B9" t="s">
-        <v>124</v>
-      </c>
-      <c r="C9" t="s">
-        <v>123</v>
-      </c>
-      <c r="D9" t="s">
-        <v>1</v>
-      </c>
-      <c r="G9" t="s">
-        <v>122</v>
-      </c>
-      <c r="H9" s="35"/>
-      <c r="J9" t="s">
-        <v>109</v>
-      </c>
-      <c r="O9" t="s">
-        <v>122</v>
-      </c>
-      <c r="P9" s="35"/>
-      <c r="Q9" t="s">
-        <v>109</v>
-      </c>
-      <c r="U9" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="10" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B10" t="s">
-        <v>122</v>
-      </c>
-      <c r="D10" t="s">
-        <v>109</v>
-      </c>
-      <c r="H10" s="35" t="s">
-        <v>108</v>
-      </c>
-      <c r="J10" t="s">
-        <v>107</v>
-      </c>
-      <c r="P10" s="36">
-        <v>41255</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="11" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="C11" s="35" t="s">
-        <v>121</v>
-      </c>
-      <c r="D11" t="s">
-        <v>109</v>
-      </c>
-      <c r="H11" s="35"/>
-      <c r="I11" t="s">
-        <v>120</v>
-      </c>
-      <c r="J11" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="12" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="C12" s="35" t="s">
-        <v>119</v>
-      </c>
-      <c r="D12" t="s">
-        <v>109</v>
-      </c>
-      <c r="H12" s="35" t="s">
-        <v>115</v>
-      </c>
-      <c r="I12" t="s">
-        <v>116</v>
-      </c>
-      <c r="J12" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="13" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="C13" s="35" t="s">
-        <v>118</v>
-      </c>
-      <c r="D13" t="s">
-        <v>109</v>
-      </c>
-      <c r="H13" s="35" t="s">
-        <v>117</v>
-      </c>
-      <c r="I13" t="s">
-        <v>116</v>
-      </c>
-      <c r="J13" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="14" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="C14" s="35" t="s">
-        <v>115</v>
-      </c>
-      <c r="D14" t="s">
-        <v>109</v>
-      </c>
-      <c r="H14" s="35" t="s">
-        <v>112</v>
-      </c>
-      <c r="I14" t="s">
-        <v>110</v>
-      </c>
-      <c r="J14" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="15" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="C15" s="35" t="s">
-        <v>114</v>
-      </c>
-      <c r="D15" t="s">
-        <v>109</v>
-      </c>
-      <c r="H15" s="35" t="s">
-        <v>113</v>
-      </c>
-      <c r="I15" t="s">
-        <v>110</v>
-      </c>
-      <c r="J15" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="16" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="C16" s="35" t="s">
-        <v>112</v>
-      </c>
-      <c r="D16" t="s">
-        <v>109</v>
-      </c>
-      <c r="H16" s="35" t="s">
-        <v>111</v>
-      </c>
-      <c r="I16" t="s">
-        <v>110</v>
-      </c>
-      <c r="J16" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="17" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C17" s="35" t="s">
-        <v>108</v>
-      </c>
-      <c r="D17" t="s">
-        <v>107</v>
-      </c>
-      <c r="H17" s="35"/>
-    </row>
-    <row r="18" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="H18" s="35"/>
-    </row>
-    <row r="19" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="H19" s="35"/>
-    </row>
-    <row r="20" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C20" s="35"/>
-      <c r="H20" s="35"/>
-    </row>
-    <row r="21" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C21" s="35"/>
-      <c r="H21" s="35"/>
-    </row>
-    <row r="22" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C22" s="35"/>
-      <c r="H22" s="35"/>
-    </row>
-    <row r="23" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C23" s="35"/>
-      <c r="H23" s="35"/>
-    </row>
-    <row r="24" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C24" s="35"/>
-      <c r="H24" s="35"/>
-    </row>
-    <row r="25" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C25" s="35"/>
-      <c r="H25" s="35"/>
-    </row>
-    <row r="26" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C26" s="35"/>
-      <c r="H26" s="35"/>
-    </row>
-    <row r="27" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C27" s="35"/>
-      <c r="H27" s="35"/>
-    </row>
-    <row r="28" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C28" s="35"/>
-      <c r="H28" s="35"/>
-    </row>
-    <row r="29" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C29" s="35"/>
-      <c r="H29" s="35"/>
-    </row>
-    <row r="30" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C30" s="35"/>
-      <c r="H30" s="35"/>
-    </row>
-    <row r="31" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C31" s="35"/>
-      <c r="H31" s="35"/>
-    </row>
-    <row r="32" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C32" s="35"/>
-      <c r="H32" s="35"/>
-    </row>
-    <row r="33" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C33" s="35"/>
-      <c r="H33" s="35"/>
-    </row>
-    <row r="34" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C34" s="35"/>
-      <c r="H34" s="35"/>
-    </row>
-    <row r="35" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="H35" s="35"/>
-    </row>
-    <row r="36" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="H36" s="35"/>
-    </row>
-    <row r="37" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="H37" s="35"/>
-    </row>
-    <row r="38" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="H38" s="35"/>
-    </row>
-  </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="G3:M3"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="U2:Y2"/>
-    <mergeCell ref="U3:Y3"/>
-    <mergeCell ref="O2:S2"/>
-    <mergeCell ref="O3:S3"/>
-    <mergeCell ref="G6:J6"/>
-    <mergeCell ref="O6:Q6"/>
-    <mergeCell ref="G2:M2"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
EPBDS-8956 removed number to Date parse logic. Rewrote tests
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/Dates.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/Dates.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\openL\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D27FD352-6E54-4AA9-BADD-C4D81C9ADD06}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="0" windowWidth="16350" windowHeight="11760" tabRatio="833" activeTab="2"/>
+    <workbookView xWindow="4455" yWindow="3000" windowWidth="21600" windowHeight="11385" tabRatio="833" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="toString" sheetId="8" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="105">
   <si>
     <t>_res_</t>
   </si>
@@ -193,12 +199,6 @@
   </si>
   <si>
     <t>Method String toStringMethod (Date date)</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>1</t>
   </si>
   <si>
     <t>05/14/1789</t>
@@ -342,7 +342,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm;@"/>
     <numFmt numFmtId="165" formatCode="h:mm:ss;@"/>
@@ -544,7 +544,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -557,10 +557,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -598,7 +596,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -960,12 +958,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="B2:D68"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D67" sqref="D67:D68"/>
+    <sheetView topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -976,22 +974,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="30"/>
+      <c r="C2" s="28"/>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="C3" s="31"/>
+      <c r="C3" s="29"/>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="C5" s="29"/>
+      <c r="C5" s="27"/>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
@@ -1013,7 +1011,7 @@
       <c r="B8" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="20" t="s">
+      <c r="C8" s="18" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1021,23 +1019,23 @@
       <c r="B9" s="5">
         <v>36892</v>
       </c>
-      <c r="C9" s="20" t="s">
+      <c r="C9" s="18" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="C10" s="20" t="s">
+      <c r="B10" s="5">
+        <v>0</v>
+      </c>
+      <c r="C10" s="18" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="C11" s="20" t="s">
+      <c r="B11" s="8">
+        <v>1</v>
+      </c>
+      <c r="C11" s="18" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1045,7 +1043,7 @@
       <c r="B12" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="20" t="s">
+      <c r="C12" s="18" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1053,7 +1051,7 @@
       <c r="B13" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="20" t="s">
+      <c r="C13" s="18" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1061,7 +1059,7 @@
       <c r="B14" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="20" t="s">
+      <c r="C14" s="18" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1069,7 +1067,7 @@
       <c r="B15" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="20" t="s">
+      <c r="C15" s="18" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1077,15 +1075,15 @@
       <c r="B16" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="20" t="s">
-        <v>63</v>
+      <c r="C16" s="18" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B17" s="15">
+      <c r="B17" s="17">
         <v>1.25</v>
       </c>
-      <c r="C17" s="20" t="s">
+      <c r="C17" s="18" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1093,93 +1091,93 @@
       <c r="B18" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="20" t="s">
+      <c r="C18" s="18" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B19" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B20" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B21" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B22" s="15">
+        <v>0.61284722222222221</v>
+      </c>
+      <c r="C22" s="18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B23" s="15">
+        <v>0.61249999999999993</v>
+      </c>
+      <c r="C23" s="18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B24" s="15">
+        <v>0.83332175925925922</v>
+      </c>
+      <c r="C24" s="18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B25" s="16">
+        <v>0.1125</v>
+      </c>
+      <c r="C25" s="18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B29" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="C29" s="28"/>
+      <c r="D29" s="28"/>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B30" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="C30" s="29"/>
+      <c r="D30" s="29"/>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B32" s="25" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B19" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="C19" s="20" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B20" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="C20" s="20" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B21" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="C21" s="20" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B22" s="17">
-        <v>0.61284722222222221</v>
-      </c>
-      <c r="C22" s="20" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B23" s="17">
-        <v>0.61249999999999993</v>
-      </c>
-      <c r="C23" s="20" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B24" s="17">
-        <v>0.83332175925925922</v>
-      </c>
-      <c r="C24" s="20" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B25" s="18">
-        <v>0.1125</v>
-      </c>
-      <c r="C25" s="20" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B29" s="30" t="s">
-        <v>66</v>
-      </c>
-      <c r="C29" s="30"/>
-      <c r="D29" s="30"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B30" s="31" t="s">
-        <v>67</v>
-      </c>
-      <c r="C30" s="31"/>
-      <c r="D30" s="31"/>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B32" s="27" t="s">
-        <v>64</v>
-      </c>
-      <c r="C32" s="28"/>
-      <c r="D32" s="29"/>
+      <c r="C32" s="26"/>
+      <c r="D32" s="27"/>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B33" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C33" s="13" t="s">
-        <v>65</v>
+      <c r="C33" s="12" t="s">
+        <v>63</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>0</v>
@@ -1189,7 +1187,7 @@
       <c r="B34" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C34" s="14" t="s">
+      <c r="C34" s="13" t="s">
         <v>4</v>
       </c>
       <c r="D34" s="4" t="s">
@@ -1198,13 +1196,13 @@
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B35" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D35" s="11" t="s">
         <v>70</v>
-      </c>
-      <c r="C35" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="D35" s="11" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.2">
@@ -1438,7 +1436,7 @@
       </c>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B58" s="19">
+      <c r="B58" s="17">
         <v>1.25</v>
       </c>
       <c r="C58" s="10" t="s">
@@ -1460,7 +1458,7 @@
       </c>
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B60" s="16" t="s">
+      <c r="B60" s="14" t="s">
         <v>33</v>
       </c>
       <c r="C60" s="10" t="s">
@@ -1471,7 +1469,7 @@
       </c>
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B61" s="16" t="s">
+      <c r="B61" s="14" t="s">
         <v>34</v>
       </c>
       <c r="C61" s="10" t="s">
@@ -1482,7 +1480,7 @@
       </c>
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B62" s="16" t="s">
+      <c r="B62" s="14" t="s">
         <v>35</v>
       </c>
       <c r="C62" s="10" t="s">
@@ -1493,7 +1491,7 @@
       </c>
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B63" s="17">
+      <c r="B63" s="15">
         <v>0.61284722222222221</v>
       </c>
       <c r="C63" s="10" t="s">
@@ -1504,7 +1502,7 @@
       </c>
     </row>
     <row r="64" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B64" s="17">
+      <c r="B64" s="15">
         <v>0.61249999999999993</v>
       </c>
       <c r="C64" s="10" t="s">
@@ -1515,7 +1513,7 @@
       </c>
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B65" s="17">
+      <c r="B65" s="15">
         <v>0.83332175925925922</v>
       </c>
       <c r="C65" s="10" t="s">
@@ -1526,7 +1524,7 @@
       </c>
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B66" s="18">
+      <c r="B66" s="16">
         <v>0.1125</v>
       </c>
       <c r="C66" s="10" t="s">
@@ -1541,7 +1539,7 @@
         <v>25</v>
       </c>
       <c r="C67" s="11" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D67" s="11" t="s">
         <v>27</v>
@@ -1552,7 +1550,7 @@
         <v>25</v>
       </c>
       <c r="C68" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D68" s="11" t="s">
         <v>28</v>
@@ -1573,11 +1571,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:E73"/>
   <sheetViews>
     <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="C96" sqref="C96"/>
+      <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1588,37 +1586,37 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B2" s="30" t="s">
-        <v>80</v>
-      </c>
-      <c r="C2" s="30"/>
+      <c r="B2" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" s="28"/>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B3" s="31" t="s">
-        <v>73</v>
-      </c>
-      <c r="C3" s="31"/>
+      <c r="B3" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" s="29"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B5" s="27" t="s">
-        <v>78</v>
-      </c>
-      <c r="C5" s="29"/>
+      <c r="B5" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="C5" s="27"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="26" t="s">
-        <v>101</v>
+      <c r="D6" s="24" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>1</v>
@@ -1628,23 +1626,23 @@
       <c r="B8" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="21">
+      <c r="C8" s="19">
         <v>42124</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="22" t="s">
+      <c r="C9" s="20" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B10" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="C10" s="21">
+        <v>74</v>
+      </c>
+      <c r="C10" s="19">
         <v>40544</v>
       </c>
     </row>
@@ -1652,7 +1650,7 @@
       <c r="B11" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="22" t="s">
+      <c r="C11" s="20" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1660,7 +1658,7 @@
       <c r="B12" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="22" t="s">
+      <c r="C12" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1668,7 +1666,7 @@
       <c r="B13" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="22" t="s">
+      <c r="C13" s="20" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1676,7 +1674,7 @@
       <c r="B14" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="22" t="s">
+      <c r="C14" s="20" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1684,23 +1682,23 @@
       <c r="B15" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="22" t="s">
-        <v>63</v>
+      <c r="C15" s="20" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B16" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="22" t="s">
-        <v>62</v>
+      <c r="C16" s="20" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B17" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="22" t="s">
+      <c r="C17" s="20" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1708,99 +1706,99 @@
       <c r="B18" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="22" t="s">
-        <v>61</v>
+      <c r="C18" s="20" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B19" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C19" s="22" t="s">
+      <c r="C19" s="20" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B20" s="22"/>
-      <c r="C20" s="22"/>
+      <c r="B20" s="20"/>
+      <c r="C20" s="20"/>
       <c r="D20" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B21" s="22" t="s">
-        <v>99</v>
-      </c>
-      <c r="C21" s="22"/>
+      <c r="B21" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="C21" s="20"/>
       <c r="D21" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B22" s="22" t="s">
-        <v>100</v>
-      </c>
-      <c r="C22" s="22"/>
+      <c r="B22" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="C22" s="20"/>
       <c r="D22" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B23" s="23"/>
-      <c r="C23" s="24"/>
+      <c r="B23" s="21"/>
+      <c r="C23" s="22"/>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B24" s="23"/>
-      <c r="C24" s="24"/>
+      <c r="B24" s="21"/>
+      <c r="C24" s="22"/>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B25" s="23"/>
-      <c r="C25" s="24"/>
+      <c r="B25" s="21"/>
+      <c r="C25" s="22"/>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B26" s="23"/>
-      <c r="C26" s="24"/>
+      <c r="B26" s="21"/>
+      <c r="C26" s="22"/>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B30" s="30" t="s">
-        <v>81</v>
-      </c>
-      <c r="C30" s="30"/>
-      <c r="D30" s="30"/>
+      <c r="B30" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="C30" s="28"/>
+      <c r="D30" s="28"/>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B31" s="31" t="s">
+      <c r="B31" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="C31" s="29"/>
+      <c r="D31" s="29"/>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B33" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="C31" s="31"/>
-      <c r="D31" s="31"/>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B33" s="27" t="s">
-        <v>79</v>
-      </c>
-      <c r="C33" s="28"/>
-      <c r="D33" s="29"/>
+      <c r="C33" s="26"/>
+      <c r="D33" s="27"/>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B34" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C34" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="D34" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="D34" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="E34" s="26" t="s">
-        <v>101</v>
+      <c r="E34" s="24" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B35" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C35" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="C35" s="13" t="s">
         <v>4</v>
       </c>
       <c r="D35" s="4" t="s">
@@ -1809,13 +1807,13 @@
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B36" s="11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D36" s="11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.2">
@@ -2001,7 +1999,7 @@
         <v>37</v>
       </c>
       <c r="D54" s="11" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.2">
@@ -2023,7 +2021,7 @@
         <v>54</v>
       </c>
       <c r="D56" s="11" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.2">
@@ -2045,7 +2043,7 @@
         <v>48</v>
       </c>
       <c r="D58" s="11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.2">
@@ -2055,7 +2053,7 @@
       <c r="C59" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D59" s="19">
+      <c r="D59" s="17">
         <v>1</v>
       </c>
     </row>
@@ -2067,7 +2065,7 @@
         <v>50</v>
       </c>
       <c r="D60" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.2">
@@ -2077,7 +2075,7 @@
       <c r="C61" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D61" s="16" t="s">
+      <c r="D61" s="14" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2088,18 +2086,18 @@
       <c r="C62" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="D62" s="16" t="s">
-        <v>87</v>
+      <c r="D62" s="14" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B63" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C63" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D63" s="16" t="s">
+      <c r="D63" s="14" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2127,7 +2125,7 @@
     </row>
     <row r="66" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B66" s="11" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C66" s="10" t="s">
         <v>51</v>
@@ -2152,7 +2150,7 @@
         <v>27</v>
       </c>
       <c r="C68" s="11" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D68" s="8" t="s">
         <v>16</v>
@@ -2163,7 +2161,7 @@
         <v>28</v>
       </c>
       <c r="C69" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D69" s="11" t="s">
         <v>16</v>
@@ -2174,43 +2172,43 @@
       <c r="C70" s="10"/>
       <c r="D70" s="10"/>
       <c r="E70" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="71" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B71" s="10" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C71" s="10" t="s">
         <v>13</v>
       </c>
       <c r="D71" s="10"/>
       <c r="E71" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="72" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B72" s="10" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C72" s="10" t="s">
         <v>37</v>
       </c>
       <c r="D72" s="10"/>
       <c r="E72" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="73" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B73" s="10" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C73" s="10" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D73" s="10"/>
       <c r="E73" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -2228,7 +2226,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B4:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -2242,36 +2240,36 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B4" s="30" t="s">
-        <v>97</v>
-      </c>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
+      <c r="B4" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B5" s="31" t="s">
-        <v>98</v>
-      </c>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
+      <c r="B5" s="29" t="s">
+        <v>96</v>
+      </c>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B7" s="32" t="s">
-        <v>93</v>
-      </c>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="34"/>
+      <c r="B7" s="30" t="s">
+        <v>91</v>
+      </c>
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="32"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="D8" s="12" t="s">
         <v>89</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>91</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>0</v>
@@ -2279,13 +2277,13 @@
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B9" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="D9" s="13" t="s">
         <v>94</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>96</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>1</v>
@@ -2302,7 +2300,7 @@
         <v>12</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.2">
@@ -2358,7 +2356,7 @@
         <v>7</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
EPBDS-12730 Date() function/constructor and suplementary functions for manipulate with Date object
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/Dates.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/Dates.xlsx
@@ -1,28 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25128"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\openL\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\openl2\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D27FD352-6E54-4AA9-BADD-C4D81C9ADD06}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EE1A4F6-6862-4561-A454-9EE4CDCC45F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4455" yWindow="3000" windowWidth="21600" windowHeight="11385" tabRatio="833" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="833" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="toString" sheetId="8" r:id="rId1"/>
     <sheet name="toDate" sheetId="11" r:id="rId2"/>
     <sheet name="Date" sheetId="10" r:id="rId3"/>
+    <sheet name="set" sheetId="12" r:id="rId4"/>
+    <sheet name="isLeap" sheetId="14" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="166">
   <si>
     <t>_res_</t>
   </si>
@@ -337,6 +339,189 @@
   </si>
   <si>
     <t>wrong input</t>
+  </si>
+  <si>
+    <t>Method Date dateMethod (int year, int month, int day, int hours, int minutes, int seconds)</t>
+  </si>
+  <si>
+    <t>hours</t>
+  </si>
+  <si>
+    <t>minutes</t>
+  </si>
+  <si>
+    <t>seconds</t>
+  </si>
+  <si>
+    <t>return Date(year, month, day, hours, minutes, seconds);</t>
+  </si>
+  <si>
+    <t>Hours</t>
+  </si>
+  <si>
+    <t>Minutes</t>
+  </si>
+  <si>
+    <t>Seconds</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>2000-1-1T2:03:04</t>
+  </si>
+  <si>
+    <t>return setTime(date, hours, minutes, seconds);</t>
+  </si>
+  <si>
+    <t>2000-1-1</t>
+  </si>
+  <si>
+    <t>7777777-1-1</t>
+  </si>
+  <si>
+    <t>1-1-1</t>
+  </si>
+  <si>
+    <t>1-1-1T23:59:59</t>
+  </si>
+  <si>
+    <t>Method Date setTimeMethod (Date date, int hours, int minutes, int seconds)</t>
+  </si>
+  <si>
+    <t>Test setTimeMethod</t>
+  </si>
+  <si>
+    <t>Method Date setTimeMethod2 (Date date, int hours, int minutes, int seconds, int milliseconds)</t>
+  </si>
+  <si>
+    <t>milliseconds</t>
+  </si>
+  <si>
+    <t>Milliseconds</t>
+  </si>
+  <si>
+    <t>7777777-1-1T00:00:00.000</t>
+  </si>
+  <si>
+    <t>2000-1-1T2:03:04.004</t>
+  </si>
+  <si>
+    <t>1-1-1T23:59:59.999</t>
+  </si>
+  <si>
+    <t>return setTime(date, hours, minutes, seconds, milliseconds);</t>
+  </si>
+  <si>
+    <t>Test setTimeMethod2</t>
+  </si>
+  <si>
+    <t>Test setDateMethod</t>
+  </si>
+  <si>
+    <t>Method Date setDateMethod (Date date, int year, int month, int day)</t>
+  </si>
+  <si>
+    <t>2000-3-4</t>
+  </si>
+  <si>
+    <t>return setDate(date, year, month, day);</t>
+  </si>
+  <si>
+    <t>return isLeap(date);</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>Method boolean isLeapMethod (Date date)</t>
+  </si>
+  <si>
+    <t>Test isLeapMethod</t>
+  </si>
+  <si>
+    <t>7777777-1-1T2:03:04.005</t>
+  </si>
+  <si>
+    <t>7777777-1-1T00:00:00.005</t>
+  </si>
+  <si>
+    <t>2000-2-1T2:03:04.005</t>
+  </si>
+  <si>
+    <t>Method Date dateMethod (int year, int month, int day, int hours, int minutes)</t>
+  </si>
+  <si>
+    <t>return Date(year, month, day, hours, minutes);</t>
+  </si>
+  <si>
+    <t>1980-07-12T12:59:00.000</t>
+  </si>
+  <si>
+    <t>2015-04-30T1:30:00.000</t>
+  </si>
+  <si>
+    <t>1-1-1T4:1:0.000</t>
+  </si>
+  <si>
+    <t>5555-12-31T5:14:00.000</t>
+  </si>
+  <si>
+    <t>7777777-07-07T22:7:00.000</t>
+  </si>
+  <si>
+    <t>1980-07-12T12:59:58.000</t>
+  </si>
+  <si>
+    <t>2015-04-30T1:30:30.000</t>
+  </si>
+  <si>
+    <t>1-1-1T4:1:1.000</t>
+  </si>
+  <si>
+    <t>5555-12-31T5:14:14.000</t>
+  </si>
+  <si>
+    <t>7777777-07-07T22:7:7.000</t>
+  </si>
+  <si>
+    <t>07/12/1980T00:00:00.000</t>
+  </si>
+  <si>
+    <t>Method Date dateMethod (int year, int month, int day, int hours, int minutes, int seconds, int milliseconds)</t>
+  </si>
+  <si>
+    <t>return Date(year, month, day, hours, minutes, seconds, milliseconds);</t>
+  </si>
+  <si>
+    <t>1980-07-12T12:59:58.004</t>
+  </si>
+  <si>
+    <t>1-1-1T4:1:1.999</t>
+  </si>
+  <si>
+    <t>5555-12-31T5:14:14.991</t>
+  </si>
+  <si>
+    <t>7777777-07-07T22:7:7.992</t>
+  </si>
+  <si>
+    <t>Method boolean isLeapMethod (Integer year)</t>
+  </si>
+  <si>
+    <t>return isLeap(year);</t>
+  </si>
+  <si>
+    <t>2000</t>
+  </si>
+  <si>
+    <t>7777777</t>
+  </si>
+  <si>
+    <t>1</t>
   </si>
 </sst>
 </file>
@@ -387,7 +572,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -514,29 +699,7 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -544,7 +707,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -570,6 +733,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -585,13 +750,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -962,36 +1127,36 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="B2:D68"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" workbookViewId="0">
+    <sheetView topLeftCell="A58" workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.5703125" customWidth="1"/>
-    <col min="3" max="3" width="26.85546875" customWidth="1"/>
-    <col min="4" max="5" width="18.28515625" customWidth="1"/>
+    <col min="2" max="2" width="19.5546875" customWidth="1"/>
+    <col min="3" max="3" width="26.88671875" customWidth="1"/>
+    <col min="4" max="5" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B2" s="28" t="s">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="28"/>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B3" s="29" t="s">
+      <c r="C2" s="30"/>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="C3" s="29"/>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B5" s="25" t="s">
+      <c r="C3" s="31"/>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="C5" s="27"/>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C5" s="29"/>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>2</v>
       </c>
@@ -999,7 +1164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>2</v>
       </c>
@@ -1007,7 +1172,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" s="11" t="s">
         <v>10</v>
       </c>
@@ -1015,7 +1180,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" s="5">
         <v>36892</v>
       </c>
@@ -1023,7 +1188,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" s="5">
         <v>0</v>
       </c>
@@ -1031,7 +1196,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" s="8">
         <v>1</v>
       </c>
@@ -1039,7 +1204,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" s="9" t="s">
         <v>6</v>
       </c>
@@ -1047,7 +1212,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" s="9" t="s">
         <v>7</v>
       </c>
@@ -1055,7 +1220,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" s="11" t="s">
         <v>8</v>
       </c>
@@ -1063,7 +1228,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B15" s="11" t="s">
         <v>5</v>
       </c>
@@ -1071,7 +1236,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B16" s="11" t="s">
         <v>31</v>
       </c>
@@ -1079,7 +1244,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="17">
         <v>1.25</v>
       </c>
@@ -1087,7 +1252,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="11" t="s">
         <v>32</v>
       </c>
@@ -1095,7 +1260,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="14" t="s">
         <v>33</v>
       </c>
@@ -1103,7 +1268,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="14" t="s">
         <v>34</v>
       </c>
@@ -1111,7 +1276,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="14" t="s">
         <v>35</v>
       </c>
@@ -1119,7 +1284,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="15">
         <v>0.61284722222222221</v>
       </c>
@@ -1127,7 +1292,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="15">
         <v>0.61249999999999993</v>
       </c>
@@ -1135,7 +1300,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="15">
         <v>0.83332175925925922</v>
       </c>
@@ -1143,7 +1308,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="16">
         <v>0.1125</v>
       </c>
@@ -1151,28 +1316,28 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B29" s="28" t="s">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B29" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="C29" s="28"/>
-      <c r="D29" s="28"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B30" s="29" t="s">
+      <c r="C29" s="30"/>
+      <c r="D29" s="30"/>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B30" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="C30" s="29"/>
-      <c r="D30" s="29"/>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B32" s="25" t="s">
+      <c r="C30" s="31"/>
+      <c r="D30" s="31"/>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B32" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="C32" s="26"/>
-      <c r="D32" s="27"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C32" s="28"/>
+      <c r="D32" s="29"/>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" s="2" t="s">
         <v>2</v>
       </c>
@@ -1183,7 +1348,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B34" s="3" t="s">
         <v>2</v>
       </c>
@@ -1194,7 +1359,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" s="11" t="s">
         <v>68</v>
       </c>
@@ -1205,7 +1370,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" s="11" t="s">
         <v>16</v>
       </c>
@@ -1216,7 +1381,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" s="11" t="s">
         <v>16</v>
       </c>
@@ -1227,7 +1392,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B38" s="11" t="s">
         <v>16</v>
       </c>
@@ -1238,7 +1403,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B39" s="11" t="s">
         <v>16</v>
       </c>
@@ -1249,7 +1414,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B40" s="11" t="s">
         <v>16</v>
       </c>
@@ -1260,7 +1425,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B41" s="11" t="s">
         <v>17</v>
       </c>
@@ -1271,7 +1436,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B42" s="11" t="s">
         <v>22</v>
       </c>
@@ -1280,7 +1445,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B43" s="11" t="s">
         <v>7</v>
       </c>
@@ -1289,7 +1454,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B44" s="11" t="s">
         <v>3</v>
       </c>
@@ -1298,7 +1463,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B45" s="11" t="s">
         <v>7</v>
       </c>
@@ -1309,7 +1474,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B46" s="11" t="s">
         <v>23</v>
       </c>
@@ -1320,7 +1485,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B47" s="9" t="s">
         <v>6</v>
       </c>
@@ -1331,7 +1496,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B48" s="11" t="s">
         <v>8</v>
       </c>
@@ -1340,7 +1505,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B49" s="11" t="s">
         <v>5</v>
       </c>
@@ -1349,7 +1514,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B50" s="11" t="s">
         <v>9</v>
       </c>
@@ -1358,7 +1523,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B51" s="11" t="s">
         <v>25</v>
       </c>
@@ -1369,7 +1534,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B52" s="9" t="s">
         <v>7</v>
       </c>
@@ -1380,7 +1545,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B53" s="11" t="s">
         <v>8</v>
       </c>
@@ -1391,7 +1556,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B54" s="11" t="s">
         <v>9</v>
       </c>
@@ -1402,7 +1567,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B55" s="11" t="s">
         <v>31</v>
       </c>
@@ -1413,7 +1578,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B56" s="11" t="s">
         <v>3</v>
       </c>
@@ -1424,7 +1589,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B57" s="11" t="s">
         <v>7</v>
       </c>
@@ -1435,7 +1600,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B58" s="17">
         <v>1.25</v>
       </c>
@@ -1446,7 +1611,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B59" s="11" t="s">
         <v>32</v>
       </c>
@@ -1457,7 +1622,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B60" s="14" t="s">
         <v>33</v>
       </c>
@@ -1468,7 +1633,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B61" s="14" t="s">
         <v>34</v>
       </c>
@@ -1479,7 +1644,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B62" s="14" t="s">
         <v>35</v>
       </c>
@@ -1490,7 +1655,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="63" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B63" s="15">
         <v>0.61284722222222221</v>
       </c>
@@ -1501,7 +1666,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="64" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B64" s="15">
         <v>0.61249999999999993</v>
       </c>
@@ -1512,7 +1677,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="65" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B65" s="15">
         <v>0.83332175925925922</v>
       </c>
@@ -1523,7 +1688,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="66" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B66" s="16">
         <v>0.1125</v>
       </c>
@@ -1534,7 +1699,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="67" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B67" s="11" t="s">
         <v>25</v>
       </c>
@@ -1545,7 +1710,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="68" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B68" s="11" t="s">
         <v>25</v>
       </c>
@@ -1574,36 +1739,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:E73"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="B64" sqref="B64"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.5703125" customWidth="1"/>
-    <col min="3" max="3" width="26.85546875" customWidth="1"/>
-    <col min="4" max="5" width="18.28515625" customWidth="1"/>
+    <col min="2" max="2" width="19.5546875" customWidth="1"/>
+    <col min="3" max="3" width="26.88671875" customWidth="1"/>
+    <col min="4" max="5" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B2" s="28" t="s">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="30" t="s">
         <v>78</v>
       </c>
-      <c r="C2" s="28"/>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B3" s="29" t="s">
+      <c r="C2" s="30"/>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="C3" s="29"/>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B5" s="25" t="s">
+      <c r="C3" s="31"/>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="27" t="s">
         <v>76</v>
       </c>
-      <c r="C5" s="27"/>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C5" s="29"/>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>72</v>
       </c>
@@ -1614,7 +1779,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>73</v>
       </c>
@@ -1622,7 +1787,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" s="11" t="s">
         <v>10</v>
       </c>
@@ -1630,7 +1795,7 @@
         <v>42124</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" s="18" t="s">
         <v>9</v>
       </c>
@@ -1638,7 +1803,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" s="11" t="s">
         <v>74</v>
       </c>
@@ -1646,7 +1811,7 @@
         <v>40544</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" s="11" t="s">
         <v>6</v>
       </c>
@@ -1654,7 +1819,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" s="11" t="s">
         <v>7</v>
       </c>
@@ -1662,7 +1827,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" s="11" t="s">
         <v>8</v>
       </c>
@@ -1670,7 +1835,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" s="11" t="s">
         <v>5</v>
       </c>
@@ -1678,7 +1843,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" s="11" t="s">
         <v>31</v>
       </c>
@@ -1686,7 +1851,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16" s="11" t="s">
         <v>32</v>
       </c>
@@ -1694,7 +1859,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="11" t="s">
         <v>33</v>
       </c>
@@ -1702,7 +1867,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="11" t="s">
         <v>34</v>
       </c>
@@ -1710,7 +1875,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="11" t="s">
         <v>35</v>
       </c>
@@ -1718,14 +1883,14 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="20"/>
       <c r="C20" s="20"/>
       <c r="D20" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="20" t="s">
         <v>97</v>
       </c>
@@ -1734,7 +1899,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="20" t="s">
         <v>98</v>
       </c>
@@ -1743,44 +1908,44 @@
         <v>104</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="21"/>
       <c r="C23" s="22"/>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="21"/>
       <c r="C24" s="22"/>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="21"/>
       <c r="C25" s="22"/>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="21"/>
       <c r="C26" s="22"/>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B30" s="28" t="s">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B30" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="C30" s="28"/>
-      <c r="D30" s="28"/>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B31" s="29" t="s">
+      <c r="C30" s="30"/>
+      <c r="D30" s="30"/>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B31" s="31" t="s">
         <v>75</v>
       </c>
-      <c r="C31" s="29"/>
-      <c r="D31" s="29"/>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B33" s="25" t="s">
+      <c r="C31" s="31"/>
+      <c r="D31" s="31"/>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B33" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="C33" s="26"/>
-      <c r="D33" s="27"/>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C33" s="28"/>
+      <c r="D33" s="29"/>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B34" s="2" t="s">
         <v>72</v>
       </c>
@@ -1794,7 +1959,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B35" s="3" t="s">
         <v>73</v>
       </c>
@@ -1805,7 +1970,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B36" s="11" t="s">
         <v>70</v>
       </c>
@@ -1816,7 +1981,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B37" s="11" t="s">
         <v>12</v>
       </c>
@@ -1827,7 +1992,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B38" s="11" t="s">
         <v>20</v>
       </c>
@@ -1838,7 +2003,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B39" s="11" t="s">
         <v>12</v>
       </c>
@@ -1849,7 +2014,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B40" s="11" t="s">
         <v>14</v>
       </c>
@@ -1860,7 +2025,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B41" s="11" t="s">
         <v>18</v>
       </c>
@@ -1871,7 +2036,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B42" s="11" t="s">
         <v>21</v>
       </c>
@@ -1882,7 +2047,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B43" s="11" t="s">
         <v>22</v>
       </c>
@@ -1891,7 +2056,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B44" s="11" t="s">
         <v>7</v>
       </c>
@@ -1900,7 +2065,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B45" s="11" t="s">
         <v>8</v>
       </c>
@@ -1909,7 +2074,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B46" s="11" t="s">
         <v>36</v>
       </c>
@@ -1920,7 +2085,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B47" s="11" t="s">
         <v>52</v>
       </c>
@@ -1931,7 +2096,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B48" s="11" t="s">
         <v>24</v>
       </c>
@@ -1942,7 +2107,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B49" s="11" t="s">
         <v>8</v>
       </c>
@@ -1951,7 +2116,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B50" s="11" t="s">
         <v>55</v>
       </c>
@@ -1960,7 +2125,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B51" s="9" t="s">
         <v>39</v>
       </c>
@@ -1969,7 +2134,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B52" s="11" t="s">
         <v>26</v>
       </c>
@@ -1980,7 +2145,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B53" s="9" t="s">
         <v>36</v>
       </c>
@@ -1991,7 +2156,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B54" s="11" t="s">
         <v>38</v>
       </c>
@@ -2002,7 +2167,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B55" s="9" t="s">
         <v>39</v>
       </c>
@@ -2013,7 +2178,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B56" s="11" t="s">
         <v>40</v>
       </c>
@@ -2024,7 +2189,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B57" s="11" t="s">
         <v>8</v>
       </c>
@@ -2035,7 +2200,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B58" s="11" t="s">
         <v>49</v>
       </c>
@@ -2046,7 +2211,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B59" s="11" t="s">
         <v>8</v>
       </c>
@@ -2057,7 +2222,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B60" s="11" t="s">
         <v>43</v>
       </c>
@@ -2068,7 +2233,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B61" s="11" t="s">
         <v>41</v>
       </c>
@@ -2079,7 +2244,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B62" s="11" t="s">
         <v>42</v>
       </c>
@@ -2090,7 +2255,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="63" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B63" s="11" t="s">
         <v>82</v>
       </c>
@@ -2101,7 +2266,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="64" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B64" s="11" t="s">
         <v>29</v>
       </c>
@@ -2112,7 +2277,7 @@
         <v>25599</v>
       </c>
     </row>
-    <row r="65" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B65" s="11" t="s">
         <v>46</v>
       </c>
@@ -2123,7 +2288,7 @@
         <v>25903</v>
       </c>
     </row>
-    <row r="66" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B66" s="11" t="s">
         <v>86</v>
       </c>
@@ -2134,7 +2299,7 @@
         <v>20090</v>
       </c>
     </row>
-    <row r="67" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B67" s="11" t="s">
         <v>36</v>
       </c>
@@ -2145,7 +2310,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="68" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B68" s="11" t="s">
         <v>27</v>
       </c>
@@ -2156,7 +2321,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="69" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B69" s="11" t="s">
         <v>28</v>
       </c>
@@ -2167,7 +2332,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="70" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B70" s="10"/>
       <c r="C70" s="10"/>
       <c r="D70" s="10"/>
@@ -2175,7 +2340,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="71" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B71" s="10" t="s">
         <v>97</v>
       </c>
@@ -2187,7 +2352,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="72" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B72" s="10" t="s">
         <v>98</v>
       </c>
@@ -2199,7 +2364,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="73" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B73" s="10" t="s">
         <v>103</v>
       </c>
@@ -2227,69 +2392,74 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="B4:E14"/>
+  <dimension ref="B4:I53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="F58" sqref="F58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="4" width="23.28515625" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" customWidth="1"/>
+    <col min="2" max="3" width="23.33203125" customWidth="1"/>
+    <col min="4" max="4" width="43.5546875" customWidth="1"/>
+    <col min="5" max="5" width="28" customWidth="1"/>
+    <col min="6" max="6" width="11.44140625" customWidth="1"/>
+    <col min="7" max="7" width="24.5546875" customWidth="1"/>
+    <col min="8" max="8" width="41.44140625" customWidth="1"/>
+    <col min="9" max="9" width="31.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B4" s="28" t="s">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B5" s="29" t="s">
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="31" t="s">
         <v>96</v>
       </c>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B7" s="30" t="s">
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="32" t="s">
         <v>91</v>
       </c>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
       <c r="E7" s="32"/>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B8" s="2" t="s">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="25" t="s">
         <v>87</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="25" t="s">
         <v>89</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="24" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B9" s="3" t="s">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="E9" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E9" s="26" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="6">
         <v>1980</v>
       </c>
@@ -2300,10 +2470,10 @@
         <v>12</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="6">
         <v>2015</v>
       </c>
@@ -2317,7 +2487,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="6">
         <v>1</v>
       </c>
@@ -2331,7 +2501,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" s="6">
         <v>5555</v>
       </c>
@@ -2345,7 +2515,7 @@
         <v>1335327</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" s="6">
         <v>7777777</v>
       </c>
@@ -2359,11 +2529,1099 @@
         <v>90</v>
       </c>
     </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="C17" s="30"/>
+      <c r="D17" s="30"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="31" t="s">
+        <v>143</v>
+      </c>
+      <c r="C18" s="31"/>
+      <c r="D18" s="31"/>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="C20" s="32"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="32"/>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="C21" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="D21" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="E21" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="F21" s="25" t="s">
+        <v>107</v>
+      </c>
+      <c r="G21" s="24" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="C22" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="D22" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="E22" s="26" t="s">
+        <v>110</v>
+      </c>
+      <c r="F22" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="G22" s="26" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="6">
+        <v>1980</v>
+      </c>
+      <c r="C23" s="6">
+        <v>7</v>
+      </c>
+      <c r="D23" s="6">
+        <v>12</v>
+      </c>
+      <c r="E23" s="6">
+        <v>12</v>
+      </c>
+      <c r="F23" s="6">
+        <v>59</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="6">
+        <v>2015</v>
+      </c>
+      <c r="C24" s="6">
+        <v>4</v>
+      </c>
+      <c r="D24" s="6">
+        <v>30</v>
+      </c>
+      <c r="E24" s="6">
+        <v>1</v>
+      </c>
+      <c r="F24" s="6">
+        <v>30</v>
+      </c>
+      <c r="G24" s="11" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="6">
+        <v>1</v>
+      </c>
+      <c r="C25" s="6">
+        <v>1</v>
+      </c>
+      <c r="D25" s="6">
+        <v>1</v>
+      </c>
+      <c r="E25" s="6">
+        <v>4</v>
+      </c>
+      <c r="F25" s="6">
+        <v>1</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="6">
+        <v>5555</v>
+      </c>
+      <c r="C26" s="6">
+        <v>12</v>
+      </c>
+      <c r="D26" s="6">
+        <v>31</v>
+      </c>
+      <c r="E26" s="6">
+        <v>5</v>
+      </c>
+      <c r="F26" s="6">
+        <v>14</v>
+      </c>
+      <c r="G26" s="11" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="6">
+        <v>7777777</v>
+      </c>
+      <c r="C27" s="6">
+        <v>7</v>
+      </c>
+      <c r="D27" s="6">
+        <v>7</v>
+      </c>
+      <c r="E27" s="6">
+        <v>22</v>
+      </c>
+      <c r="F27" s="6">
+        <v>7</v>
+      </c>
+      <c r="G27" s="11" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="C30" s="30"/>
+      <c r="D30" s="30"/>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B31" s="31" t="s">
+        <v>109</v>
+      </c>
+      <c r="C31" s="31"/>
+      <c r="D31" s="31"/>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B33" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="C33" s="32"/>
+      <c r="D33" s="32"/>
+      <c r="E33" s="32"/>
+      <c r="F33" s="32"/>
+      <c r="G33" s="32"/>
+      <c r="H33" s="32"/>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B34" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="C34" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="D34" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="E34" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="F34" s="25" t="s">
+        <v>107</v>
+      </c>
+      <c r="G34" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="H34" s="24" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B35" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="C35" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="D35" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="E35" s="26" t="s">
+        <v>110</v>
+      </c>
+      <c r="F35" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="G35" s="26" t="s">
+        <v>112</v>
+      </c>
+      <c r="H35" s="26" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B36" s="6">
+        <v>1980</v>
+      </c>
+      <c r="C36" s="6">
+        <v>7</v>
+      </c>
+      <c r="D36" s="6">
+        <v>12</v>
+      </c>
+      <c r="E36" s="6">
+        <v>12</v>
+      </c>
+      <c r="F36" s="6">
+        <v>59</v>
+      </c>
+      <c r="G36" s="6">
+        <v>58</v>
+      </c>
+      <c r="H36" s="11" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B37" s="6">
+        <v>2015</v>
+      </c>
+      <c r="C37" s="6">
+        <v>4</v>
+      </c>
+      <c r="D37" s="6">
+        <v>30</v>
+      </c>
+      <c r="E37" s="6">
+        <v>1</v>
+      </c>
+      <c r="F37" s="6">
+        <v>30</v>
+      </c>
+      <c r="G37" s="6">
+        <v>30</v>
+      </c>
+      <c r="H37" s="11" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B38" s="6">
+        <v>1</v>
+      </c>
+      <c r="C38" s="6">
+        <v>1</v>
+      </c>
+      <c r="D38" s="6">
+        <v>1</v>
+      </c>
+      <c r="E38" s="6">
+        <v>4</v>
+      </c>
+      <c r="F38" s="6">
+        <v>1</v>
+      </c>
+      <c r="G38" s="6">
+        <v>1</v>
+      </c>
+      <c r="H38" s="11" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B39" s="6">
+        <v>5555</v>
+      </c>
+      <c r="C39" s="6">
+        <v>12</v>
+      </c>
+      <c r="D39" s="6">
+        <v>31</v>
+      </c>
+      <c r="E39" s="6">
+        <v>5</v>
+      </c>
+      <c r="F39" s="6">
+        <v>14</v>
+      </c>
+      <c r="G39" s="6">
+        <v>14</v>
+      </c>
+      <c r="H39" s="11" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B40" s="6">
+        <v>7777777</v>
+      </c>
+      <c r="C40" s="6">
+        <v>7</v>
+      </c>
+      <c r="D40" s="6">
+        <v>7</v>
+      </c>
+      <c r="E40" s="6">
+        <v>22</v>
+      </c>
+      <c r="F40" s="6">
+        <v>7</v>
+      </c>
+      <c r="G40" s="6">
+        <v>7</v>
+      </c>
+      <c r="H40" s="11" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B43" s="30" t="s">
+        <v>155</v>
+      </c>
+      <c r="C43" s="30"/>
+      <c r="D43" s="30"/>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B44" s="31" t="s">
+        <v>156</v>
+      </c>
+      <c r="C44" s="31"/>
+      <c r="D44" s="31"/>
+    </row>
+    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B46" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="C46" s="32"/>
+      <c r="D46" s="32"/>
+      <c r="E46" s="32"/>
+      <c r="F46" s="32"/>
+      <c r="G46" s="32"/>
+      <c r="H46" s="32"/>
+    </row>
+    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B47" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="C47" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="D47" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="E47" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="F47" s="25" t="s">
+        <v>107</v>
+      </c>
+      <c r="G47" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="H47" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="I47" s="24" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B48" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="C48" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="D48" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="E48" s="26" t="s">
+        <v>110</v>
+      </c>
+      <c r="F48" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="G48" s="26" t="s">
+        <v>112</v>
+      </c>
+      <c r="H48" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="I48" s="26" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B49" s="6">
+        <v>1980</v>
+      </c>
+      <c r="C49" s="6">
+        <v>7</v>
+      </c>
+      <c r="D49" s="6">
+        <v>12</v>
+      </c>
+      <c r="E49" s="6">
+        <v>12</v>
+      </c>
+      <c r="F49" s="6">
+        <v>59</v>
+      </c>
+      <c r="G49" s="6">
+        <v>58</v>
+      </c>
+      <c r="H49" s="6">
+        <v>4</v>
+      </c>
+      <c r="I49" s="11" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B50" s="6">
+        <v>2015</v>
+      </c>
+      <c r="C50" s="6">
+        <v>4</v>
+      </c>
+      <c r="D50" s="6">
+        <v>30</v>
+      </c>
+      <c r="E50" s="6">
+        <v>1</v>
+      </c>
+      <c r="F50" s="6">
+        <v>30</v>
+      </c>
+      <c r="G50" s="6">
+        <v>30</v>
+      </c>
+      <c r="H50" s="6">
+        <v>0</v>
+      </c>
+      <c r="I50" s="11" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B51" s="6">
+        <v>1</v>
+      </c>
+      <c r="C51" s="6">
+        <v>1</v>
+      </c>
+      <c r="D51" s="6">
+        <v>1</v>
+      </c>
+      <c r="E51" s="6">
+        <v>4</v>
+      </c>
+      <c r="F51" s="6">
+        <v>1</v>
+      </c>
+      <c r="G51" s="6">
+        <v>1</v>
+      </c>
+      <c r="H51" s="6">
+        <v>999</v>
+      </c>
+      <c r="I51" s="11" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B52" s="6">
+        <v>5555</v>
+      </c>
+      <c r="C52" s="6">
+        <v>12</v>
+      </c>
+      <c r="D52" s="6">
+        <v>31</v>
+      </c>
+      <c r="E52" s="6">
+        <v>5</v>
+      </c>
+      <c r="F52" s="6">
+        <v>14</v>
+      </c>
+      <c r="G52" s="6">
+        <v>14</v>
+      </c>
+      <c r="H52" s="6">
+        <v>991</v>
+      </c>
+      <c r="I52" s="11" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B53" s="6">
+        <v>7777777</v>
+      </c>
+      <c r="C53" s="6">
+        <v>7</v>
+      </c>
+      <c r="D53" s="6">
+        <v>7</v>
+      </c>
+      <c r="E53" s="6">
+        <v>22</v>
+      </c>
+      <c r="F53" s="6">
+        <v>7</v>
+      </c>
+      <c r="G53" s="6">
+        <v>7</v>
+      </c>
+      <c r="H53" s="6">
+        <v>992</v>
+      </c>
+      <c r="I53" s="11" t="s">
+        <v>160</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="12">
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="B46:H46"/>
+    <mergeCell ref="B33:H33"/>
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B20:G20"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ECBA2BC-33CC-4577-BDBD-94A2E6F0BB52}">
+  <dimension ref="B4:G38"/>
+  <sheetViews>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22:F26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="23.33203125" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" customWidth="1"/>
+    <col min="4" max="4" width="40.21875" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" customWidth="1"/>
+    <col min="6" max="6" width="23.88671875" customWidth="1"/>
+    <col min="7" max="7" width="28.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="30" t="s">
+        <v>120</v>
+      </c>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="31" t="s">
+        <v>115</v>
+      </c>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="33" t="s">
+        <v>121</v>
+      </c>
+      <c r="C8" s="34"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="C11" s="6">
+        <v>2</v>
+      </c>
+      <c r="D11" s="6">
+        <v>3</v>
+      </c>
+      <c r="E11" s="6">
+        <v>4</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="C12" s="6">
+        <v>0</v>
+      </c>
+      <c r="D12" s="6">
+        <v>0</v>
+      </c>
+      <c r="E12" s="6">
+        <v>0</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="C13" s="6">
+        <v>23</v>
+      </c>
+      <c r="D13" s="6">
+        <v>59</v>
+      </c>
+      <c r="E13" s="6">
+        <v>59</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="30" t="s">
+        <v>122</v>
+      </c>
+      <c r="C17" s="30"/>
+      <c r="D17" s="30"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="31" t="s">
+        <v>128</v>
+      </c>
+      <c r="C18" s="31"/>
+      <c r="D18" s="31"/>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="33" t="s">
+        <v>129</v>
+      </c>
+      <c r="C21" s="34"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="34"/>
+      <c r="F21" s="34"/>
+      <c r="G21" s="34"/>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="E23" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="F23" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="C24" s="6">
+        <v>2</v>
+      </c>
+      <c r="D24" s="6">
+        <v>3</v>
+      </c>
+      <c r="E24" s="6">
+        <v>4</v>
+      </c>
+      <c r="F24" s="6">
+        <v>4</v>
+      </c>
+      <c r="G24" s="11" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="C25" s="6">
+        <v>0</v>
+      </c>
+      <c r="D25" s="6">
+        <v>0</v>
+      </c>
+      <c r="E25" s="6">
+        <v>0</v>
+      </c>
+      <c r="F25" s="6">
+        <v>0</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="C26" s="6">
+        <v>23</v>
+      </c>
+      <c r="D26" s="6">
+        <v>59</v>
+      </c>
+      <c r="E26" s="6">
+        <v>59</v>
+      </c>
+      <c r="F26" s="6">
+        <v>999</v>
+      </c>
+      <c r="G26" s="11" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B29" s="30" t="s">
+        <v>131</v>
+      </c>
+      <c r="C29" s="30"/>
+      <c r="D29" s="30"/>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="31" t="s">
+        <v>133</v>
+      </c>
+      <c r="C30" s="31"/>
+      <c r="D30" s="31"/>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B33" s="33" t="s">
+        <v>130</v>
+      </c>
+      <c r="C33" s="34"/>
+      <c r="D33" s="34"/>
+      <c r="E33" s="34"/>
+      <c r="F33" s="34"/>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B34" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D34" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="E34" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B35" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D35" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="E35" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B36" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="C36" s="6">
+        <v>2000</v>
+      </c>
+      <c r="D36" s="6">
+        <v>3</v>
+      </c>
+      <c r="E36" s="6">
+        <v>4</v>
+      </c>
+      <c r="F36" s="11" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B37" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="C37" s="6">
+        <v>2000</v>
+      </c>
+      <c r="D37" s="6">
+        <v>2</v>
+      </c>
+      <c r="E37" s="6">
+        <v>1</v>
+      </c>
+      <c r="F37" s="11" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B38" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="C38" s="6">
+        <v>1</v>
+      </c>
+      <c r="D38" s="6">
+        <v>1</v>
+      </c>
+      <c r="E38" s="6">
+        <v>1</v>
+      </c>
+      <c r="F38" s="11" t="s">
+        <v>127</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B33:F33"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B18:D18"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7ED34E8-D060-402C-99E7-2BC0710CBE80}">
+  <dimension ref="B4:D24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="28.109375" customWidth="1"/>
+    <col min="3" max="3" width="26" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4" s="30" t="s">
+        <v>137</v>
+      </c>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="31" t="s">
+        <v>134</v>
+      </c>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="33" t="s">
+        <v>138</v>
+      </c>
+      <c r="C7" s="34"/>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B16" s="30" t="s">
+        <v>161</v>
+      </c>
+      <c r="C16" s="30"/>
+      <c r="D16" s="30"/>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="31" t="s">
+        <v>162</v>
+      </c>
+      <c r="C17" s="31"/>
+      <c r="D17" s="31"/>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="33" t="s">
+        <v>138</v>
+      </c>
+      <c r="C19" s="34"/>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>136</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B17:D17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
EPBDS-12730 Date() function/constructor and suplementary functions for manipulate with Date object (#491)
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/Dates.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/Dates.xlsx
@@ -1,28 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10611"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\openL\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ekosolapova/work/demoEPBDS-12730/openl-demo/user-workspace/DEFAULT/Dates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D27FD352-6E54-4AA9-BADD-C4D81C9ADD06}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D0463A8-79EA-5744-AFE1-139DE74D3D77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4455" yWindow="3000" windowWidth="21600" windowHeight="11385" tabRatio="833" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1240" yWindow="500" windowWidth="37160" windowHeight="21160" tabRatio="833" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="toString" sheetId="8" r:id="rId1"/>
     <sheet name="toDate" sheetId="11" r:id="rId2"/>
     <sheet name="Date" sheetId="10" r:id="rId3"/>
+    <sheet name="set" sheetId="12" r:id="rId4"/>
+    <sheet name="isLeap" sheetId="14" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="173">
   <si>
     <t>_res_</t>
   </si>
@@ -337,6 +339,210 @@
   </si>
   <si>
     <t>wrong input</t>
+  </si>
+  <si>
+    <t>Method Date dateMethod (int year, int month, int day, int hours, int minutes, int seconds)</t>
+  </si>
+  <si>
+    <t>hours</t>
+  </si>
+  <si>
+    <t>minutes</t>
+  </si>
+  <si>
+    <t>seconds</t>
+  </si>
+  <si>
+    <t>return Date(year, month, day, hours, minutes, seconds);</t>
+  </si>
+  <si>
+    <t>Hours</t>
+  </si>
+  <si>
+    <t>Minutes</t>
+  </si>
+  <si>
+    <t>Seconds</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>2000-1-1T2:03:04</t>
+  </si>
+  <si>
+    <t>return setTime(date, hours, minutes, seconds);</t>
+  </si>
+  <si>
+    <t>2000-1-1</t>
+  </si>
+  <si>
+    <t>7777777-1-1</t>
+  </si>
+  <si>
+    <t>1-1-1</t>
+  </si>
+  <si>
+    <t>1-1-1T23:59:59</t>
+  </si>
+  <si>
+    <t>Method Date setTimeMethod (Date date, int hours, int minutes, int seconds)</t>
+  </si>
+  <si>
+    <t>Test setTimeMethod</t>
+  </si>
+  <si>
+    <t>Method Date setTimeMethod2 (Date date, int hours, int minutes, int seconds, int milliseconds)</t>
+  </si>
+  <si>
+    <t>milliseconds</t>
+  </si>
+  <si>
+    <t>Milliseconds</t>
+  </si>
+  <si>
+    <t>7777777-1-1T00:00:00.000</t>
+  </si>
+  <si>
+    <t>2000-1-1T2:03:04.004</t>
+  </si>
+  <si>
+    <t>1-1-1T23:59:59.999</t>
+  </si>
+  <si>
+    <t>return setTime(date, hours, minutes, seconds, milliseconds);</t>
+  </si>
+  <si>
+    <t>Test setTimeMethod2</t>
+  </si>
+  <si>
+    <t>Test setDateMethod</t>
+  </si>
+  <si>
+    <t>Method Date setDateMethod (Date date, int year, int month, int day)</t>
+  </si>
+  <si>
+    <t>2000-3-4</t>
+  </si>
+  <si>
+    <t>return setDate(date, year, month, day);</t>
+  </si>
+  <si>
+    <t>return isLeap(date);</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>Method boolean isLeapMethod (Date date)</t>
+  </si>
+  <si>
+    <t>Test isLeapMethod</t>
+  </si>
+  <si>
+    <t>7777777-1-1T2:03:04.005</t>
+  </si>
+  <si>
+    <t>7777777-1-1T00:00:00.005</t>
+  </si>
+  <si>
+    <t>2000-2-1T2:03:04.005</t>
+  </si>
+  <si>
+    <t>Method Date dateMethod (int year, int month, int day, int hours, int minutes)</t>
+  </si>
+  <si>
+    <t>return Date(year, month, day, hours, minutes);</t>
+  </si>
+  <si>
+    <t>1980-07-12T12:59:00.000</t>
+  </si>
+  <si>
+    <t>2015-04-30T1:30:00.000</t>
+  </si>
+  <si>
+    <t>1-1-1T4:1:0.000</t>
+  </si>
+  <si>
+    <t>5555-12-31T5:14:00.000</t>
+  </si>
+  <si>
+    <t>7777777-07-07T22:7:00.000</t>
+  </si>
+  <si>
+    <t>1980-07-12T12:59:58.000</t>
+  </si>
+  <si>
+    <t>2015-04-30T1:30:30.000</t>
+  </si>
+  <si>
+    <t>1-1-1T4:1:1.000</t>
+  </si>
+  <si>
+    <t>5555-12-31T5:14:14.000</t>
+  </si>
+  <si>
+    <t>7777777-07-07T22:7:7.000</t>
+  </si>
+  <si>
+    <t>07/12/1980T00:00:00.000</t>
+  </si>
+  <si>
+    <t>Method Date dateMethod (int year, int month, int day, int hours, int minutes, int seconds, int milliseconds)</t>
+  </si>
+  <si>
+    <t>return Date(year, month, day, hours, minutes, seconds, milliseconds);</t>
+  </si>
+  <si>
+    <t>1980-07-12T12:59:58.004</t>
+  </si>
+  <si>
+    <t>1-1-1T4:1:1.999</t>
+  </si>
+  <si>
+    <t>5555-12-31T5:14:14.991</t>
+  </si>
+  <si>
+    <t>7777777-07-07T22:7:7.992</t>
+  </si>
+  <si>
+    <t>Method boolean isLeapMethod (Integer year)</t>
+  </si>
+  <si>
+    <t>return isLeap(year);</t>
+  </si>
+  <si>
+    <t>2000</t>
+  </si>
+  <si>
+    <t>7777777</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>return setTime(date, hours, minutes);</t>
+  </si>
+  <si>
+    <t>Test setTimeMethod3</t>
+  </si>
+  <si>
+    <t>Method Date setTimeMethod3(Date date, int hours, int minutes)</t>
+  </si>
+  <si>
+    <t>2000-1-1T2:03:00</t>
+  </si>
+  <si>
+    <t>1-1-1T23:59:00</t>
+  </si>
+  <si>
+    <t>7777777-1-1T00:00:04.005</t>
+  </si>
+  <si>
+    <t>//negatove tests</t>
   </si>
 </sst>
 </file>
@@ -387,7 +593,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -514,6 +720,15 @@
         <color indexed="64"/>
       </left>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -540,11 +755,44 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -570,6 +818,26 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -585,18 +853,27 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -962,36 +1239,36 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="B2:D68"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="19.5703125" customWidth="1"/>
-    <col min="3" max="3" width="26.85546875" customWidth="1"/>
-    <col min="4" max="5" width="18.28515625" customWidth="1"/>
+    <col min="2" max="2" width="19.5" customWidth="1"/>
+    <col min="3" max="3" width="26.83203125" customWidth="1"/>
+    <col min="4" max="5" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B2" s="28" t="s">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B2" s="48" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="28"/>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B3" s="29" t="s">
+      <c r="C2" s="48"/>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B3" s="49" t="s">
         <v>56</v>
       </c>
-      <c r="C3" s="29"/>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B5" s="25" t="s">
+      <c r="C3" s="49"/>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B5" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="C5" s="27"/>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C5" s="47"/>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B6" s="2" t="s">
         <v>2</v>
       </c>
@@ -999,7 +1276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B7" s="3" t="s">
         <v>2</v>
       </c>
@@ -1007,7 +1284,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B8" s="11" t="s">
         <v>10</v>
       </c>
@@ -1015,7 +1292,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B9" s="5">
         <v>36892</v>
       </c>
@@ -1023,7 +1300,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B10" s="5">
         <v>0</v>
       </c>
@@ -1031,7 +1308,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B11" s="8">
         <v>1</v>
       </c>
@@ -1039,7 +1316,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B12" s="9" t="s">
         <v>6</v>
       </c>
@@ -1047,7 +1324,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B13" s="9" t="s">
         <v>7</v>
       </c>
@@ -1055,7 +1332,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B14" s="11" t="s">
         <v>8</v>
       </c>
@@ -1063,7 +1340,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B15" s="11" t="s">
         <v>5</v>
       </c>
@@ -1071,7 +1348,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B16" s="11" t="s">
         <v>31</v>
       </c>
@@ -1079,7 +1356,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B17" s="17">
         <v>1.25</v>
       </c>
@@ -1087,7 +1364,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B18" s="11" t="s">
         <v>32</v>
       </c>
@@ -1095,7 +1372,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B19" s="14" t="s">
         <v>33</v>
       </c>
@@ -1103,7 +1380,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B20" s="14" t="s">
         <v>34</v>
       </c>
@@ -1111,7 +1388,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B21" s="14" t="s">
         <v>35</v>
       </c>
@@ -1119,7 +1396,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B22" s="15">
         <v>0.61284722222222221</v>
       </c>
@@ -1127,7 +1404,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B23" s="15">
         <v>0.61249999999999993</v>
       </c>
@@ -1135,7 +1412,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B24" s="15">
         <v>0.83332175925925922</v>
       </c>
@@ -1143,7 +1420,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B25" s="16">
         <v>0.1125</v>
       </c>
@@ -1151,28 +1428,28 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B29" s="28" t="s">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B29" s="48" t="s">
         <v>64</v>
       </c>
-      <c r="C29" s="28"/>
-      <c r="D29" s="28"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B30" s="29" t="s">
+      <c r="C29" s="48"/>
+      <c r="D29" s="48"/>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B30" s="49" t="s">
         <v>65</v>
       </c>
-      <c r="C30" s="29"/>
-      <c r="D30" s="29"/>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B32" s="25" t="s">
+      <c r="C30" s="49"/>
+      <c r="D30" s="49"/>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B32" s="45" t="s">
         <v>62</v>
       </c>
-      <c r="C32" s="26"/>
-      <c r="D32" s="27"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C32" s="46"/>
+      <c r="D32" s="47"/>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B33" s="2" t="s">
         <v>2</v>
       </c>
@@ -1183,7 +1460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B34" s="3" t="s">
         <v>2</v>
       </c>
@@ -1194,7 +1471,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B35" s="11" t="s">
         <v>68</v>
       </c>
@@ -1205,7 +1482,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B36" s="11" t="s">
         <v>16</v>
       </c>
@@ -1216,7 +1493,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B37" s="11" t="s">
         <v>16</v>
       </c>
@@ -1227,7 +1504,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B38" s="11" t="s">
         <v>16</v>
       </c>
@@ -1238,7 +1515,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B39" s="11" t="s">
         <v>16</v>
       </c>
@@ -1249,7 +1526,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B40" s="11" t="s">
         <v>16</v>
       </c>
@@ -1260,7 +1537,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B41" s="11" t="s">
         <v>17</v>
       </c>
@@ -1271,7 +1548,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B42" s="11" t="s">
         <v>22</v>
       </c>
@@ -1280,7 +1557,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B43" s="11" t="s">
         <v>7</v>
       </c>
@@ -1289,7 +1566,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B44" s="11" t="s">
         <v>3</v>
       </c>
@@ -1298,7 +1575,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B45" s="11" t="s">
         <v>7</v>
       </c>
@@ -1309,7 +1586,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B46" s="11" t="s">
         <v>23</v>
       </c>
@@ -1320,7 +1597,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B47" s="9" t="s">
         <v>6</v>
       </c>
@@ -1331,7 +1608,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B48" s="11" t="s">
         <v>8</v>
       </c>
@@ -1340,7 +1617,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B49" s="11" t="s">
         <v>5</v>
       </c>
@@ -1349,7 +1626,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B50" s="11" t="s">
         <v>9</v>
       </c>
@@ -1358,7 +1635,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B51" s="11" t="s">
         <v>25</v>
       </c>
@@ -1369,7 +1646,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B52" s="9" t="s">
         <v>7</v>
       </c>
@@ -1380,7 +1657,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B53" s="11" t="s">
         <v>8</v>
       </c>
@@ -1391,7 +1668,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B54" s="11" t="s">
         <v>9</v>
       </c>
@@ -1402,7 +1679,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B55" s="11" t="s">
         <v>31</v>
       </c>
@@ -1413,7 +1690,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B56" s="11" t="s">
         <v>3</v>
       </c>
@@ -1424,7 +1701,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B57" s="11" t="s">
         <v>7</v>
       </c>
@@ -1435,7 +1712,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B58" s="17">
         <v>1.25</v>
       </c>
@@ -1446,7 +1723,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B59" s="11" t="s">
         <v>32</v>
       </c>
@@ -1457,7 +1734,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B60" s="14" t="s">
         <v>33</v>
       </c>
@@ -1468,7 +1745,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B61" s="14" t="s">
         <v>34</v>
       </c>
@@ -1479,7 +1756,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B62" s="14" t="s">
         <v>35</v>
       </c>
@@ -1490,7 +1767,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="63" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B63" s="15">
         <v>0.61284722222222221</v>
       </c>
@@ -1501,7 +1778,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="64" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B64" s="15">
         <v>0.61249999999999993</v>
       </c>
@@ -1512,7 +1789,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="65" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B65" s="15">
         <v>0.83332175925925922</v>
       </c>
@@ -1523,7 +1800,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="66" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B66" s="16">
         <v>0.1125</v>
       </c>
@@ -1534,7 +1811,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="67" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B67" s="11" t="s">
         <v>25</v>
       </c>
@@ -1545,7 +1822,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="68" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B68" s="11" t="s">
         <v>25</v>
       </c>
@@ -1574,36 +1851,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:E73"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="B64" sqref="B64"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="19.5703125" customWidth="1"/>
-    <col min="3" max="3" width="26.85546875" customWidth="1"/>
-    <col min="4" max="5" width="18.28515625" customWidth="1"/>
+    <col min="2" max="2" width="19.5" customWidth="1"/>
+    <col min="3" max="3" width="26.83203125" customWidth="1"/>
+    <col min="4" max="5" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B2" s="28" t="s">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B2" s="48" t="s">
         <v>78</v>
       </c>
-      <c r="C2" s="28"/>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B3" s="29" t="s">
+      <c r="C2" s="48"/>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B3" s="49" t="s">
         <v>71</v>
       </c>
-      <c r="C3" s="29"/>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B5" s="25" t="s">
+      <c r="C3" s="49"/>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B5" s="45" t="s">
         <v>76</v>
       </c>
-      <c r="C5" s="27"/>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C5" s="47"/>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B6" s="2" t="s">
         <v>72</v>
       </c>
@@ -1614,7 +1891,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B7" s="3" t="s">
         <v>73</v>
       </c>
@@ -1622,7 +1899,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B8" s="11" t="s">
         <v>10</v>
       </c>
@@ -1630,7 +1907,7 @@
         <v>42124</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B9" s="18" t="s">
         <v>9</v>
       </c>
@@ -1638,7 +1915,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B10" s="11" t="s">
         <v>74</v>
       </c>
@@ -1646,7 +1923,7 @@
         <v>40544</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B11" s="11" t="s">
         <v>6</v>
       </c>
@@ -1654,7 +1931,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B12" s="11" t="s">
         <v>7</v>
       </c>
@@ -1662,7 +1939,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B13" s="11" t="s">
         <v>8</v>
       </c>
@@ -1670,7 +1947,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B14" s="11" t="s">
         <v>5</v>
       </c>
@@ -1678,7 +1955,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B15" s="11" t="s">
         <v>31</v>
       </c>
@@ -1686,7 +1963,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B16" s="11" t="s">
         <v>32</v>
       </c>
@@ -1694,7 +1971,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B17" s="11" t="s">
         <v>33</v>
       </c>
@@ -1702,7 +1979,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B18" s="11" t="s">
         <v>34</v>
       </c>
@@ -1710,7 +1987,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B19" s="11" t="s">
         <v>35</v>
       </c>
@@ -1718,14 +1995,14 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B20" s="20"/>
       <c r="C20" s="20"/>
       <c r="D20" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B21" s="20" t="s">
         <v>97</v>
       </c>
@@ -1734,7 +2011,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B22" s="20" t="s">
         <v>98</v>
       </c>
@@ -1743,44 +2020,44 @@
         <v>104</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B23" s="21"/>
       <c r="C23" s="22"/>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B24" s="21"/>
       <c r="C24" s="22"/>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B25" s="21"/>
       <c r="C25" s="22"/>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B26" s="21"/>
       <c r="C26" s="22"/>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B30" s="28" t="s">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B30" s="48" t="s">
         <v>79</v>
       </c>
-      <c r="C30" s="28"/>
-      <c r="D30" s="28"/>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B31" s="29" t="s">
+      <c r="C30" s="48"/>
+      <c r="D30" s="48"/>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B31" s="49" t="s">
         <v>75</v>
       </c>
-      <c r="C31" s="29"/>
-      <c r="D31" s="29"/>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B33" s="25" t="s">
+      <c r="C31" s="49"/>
+      <c r="D31" s="49"/>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B33" s="45" t="s">
         <v>77</v>
       </c>
-      <c r="C33" s="26"/>
-      <c r="D33" s="27"/>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C33" s="46"/>
+      <c r="D33" s="47"/>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B34" s="2" t="s">
         <v>72</v>
       </c>
@@ -1794,7 +2071,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B35" s="3" t="s">
         <v>73</v>
       </c>
@@ -1805,7 +2082,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B36" s="11" t="s">
         <v>70</v>
       </c>
@@ -1816,7 +2093,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B37" s="11" t="s">
         <v>12</v>
       </c>
@@ -1827,7 +2104,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B38" s="11" t="s">
         <v>20</v>
       </c>
@@ -1838,7 +2115,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B39" s="11" t="s">
         <v>12</v>
       </c>
@@ -1849,7 +2126,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B40" s="11" t="s">
         <v>14</v>
       </c>
@@ -1860,7 +2137,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B41" s="11" t="s">
         <v>18</v>
       </c>
@@ -1871,7 +2148,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B42" s="11" t="s">
         <v>21</v>
       </c>
@@ -1882,7 +2159,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B43" s="11" t="s">
         <v>22</v>
       </c>
@@ -1891,7 +2168,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B44" s="11" t="s">
         <v>7</v>
       </c>
@@ -1900,7 +2177,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B45" s="11" t="s">
         <v>8</v>
       </c>
@@ -1909,7 +2186,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B46" s="11" t="s">
         <v>36</v>
       </c>
@@ -1920,7 +2197,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B47" s="11" t="s">
         <v>52</v>
       </c>
@@ -1931,7 +2208,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B48" s="11" t="s">
         <v>24</v>
       </c>
@@ -1942,7 +2219,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B49" s="11" t="s">
         <v>8</v>
       </c>
@@ -1951,7 +2228,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B50" s="11" t="s">
         <v>55</v>
       </c>
@@ -1960,7 +2237,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B51" s="9" t="s">
         <v>39</v>
       </c>
@@ -1969,7 +2246,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B52" s="11" t="s">
         <v>26</v>
       </c>
@@ -1980,7 +2257,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B53" s="9" t="s">
         <v>36</v>
       </c>
@@ -1991,7 +2268,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B54" s="11" t="s">
         <v>38</v>
       </c>
@@ -2002,7 +2279,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B55" s="9" t="s">
         <v>39</v>
       </c>
@@ -2013,7 +2290,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B56" s="11" t="s">
         <v>40</v>
       </c>
@@ -2024,7 +2301,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B57" s="11" t="s">
         <v>8</v>
       </c>
@@ -2035,7 +2312,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B58" s="11" t="s">
         <v>49</v>
       </c>
@@ -2046,7 +2323,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B59" s="11" t="s">
         <v>8</v>
       </c>
@@ -2057,7 +2334,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B60" s="11" t="s">
         <v>43</v>
       </c>
@@ -2068,7 +2345,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B61" s="11" t="s">
         <v>41</v>
       </c>
@@ -2079,7 +2356,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B62" s="11" t="s">
         <v>42</v>
       </c>
@@ -2090,7 +2367,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="63" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B63" s="11" t="s">
         <v>82</v>
       </c>
@@ -2101,7 +2378,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="64" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B64" s="11" t="s">
         <v>29</v>
       </c>
@@ -2112,7 +2389,7 @@
         <v>25599</v>
       </c>
     </row>
-    <row r="65" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B65" s="11" t="s">
         <v>46</v>
       </c>
@@ -2123,7 +2400,7 @@
         <v>25903</v>
       </c>
     </row>
-    <row r="66" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B66" s="11" t="s">
         <v>86</v>
       </c>
@@ -2134,7 +2411,7 @@
         <v>20090</v>
       </c>
     </row>
-    <row r="67" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B67" s="11" t="s">
         <v>36</v>
       </c>
@@ -2145,7 +2422,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="68" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B68" s="11" t="s">
         <v>27</v>
       </c>
@@ -2156,7 +2433,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="69" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B69" s="11" t="s">
         <v>28</v>
       </c>
@@ -2167,7 +2444,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="70" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B70" s="10"/>
       <c r="C70" s="10"/>
       <c r="D70" s="10"/>
@@ -2175,7 +2452,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="71" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B71" s="10" t="s">
         <v>97</v>
       </c>
@@ -2187,7 +2464,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="72" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B72" s="10" t="s">
         <v>98</v>
       </c>
@@ -2199,7 +2476,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="73" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B73" s="10" t="s">
         <v>103</v>
       </c>
@@ -2227,69 +2504,74 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="B4:E14"/>
+  <dimension ref="B4:K126"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="I115" sqref="I115:I126"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="4" width="23.28515625" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" customWidth="1"/>
+    <col min="2" max="3" width="23.33203125" customWidth="1"/>
+    <col min="4" max="4" width="43.5" customWidth="1"/>
+    <col min="5" max="5" width="28" customWidth="1"/>
+    <col min="6" max="6" width="11.5" customWidth="1"/>
+    <col min="7" max="7" width="24.5" customWidth="1"/>
+    <col min="8" max="8" width="41.5" customWidth="1"/>
+    <col min="9" max="9" width="31.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B4" s="28" t="s">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B4" s="48" t="s">
         <v>95</v>
       </c>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B5" s="29" t="s">
+      <c r="C4" s="48"/>
+      <c r="D4" s="48"/>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B5" s="49" t="s">
         <v>96</v>
       </c>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B7" s="30" t="s">
+      <c r="C5" s="49"/>
+      <c r="D5" s="49"/>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B7" s="50" t="s">
         <v>91</v>
       </c>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="32"/>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B8" s="2" t="s">
+      <c r="C7" s="50"/>
+      <c r="D7" s="50"/>
+      <c r="E7" s="50"/>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B8" s="25" t="s">
         <v>87</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="25" t="s">
         <v>89</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="24" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B9" s="3" t="s">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B9" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="E9" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E9" s="26" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B10" s="6">
         <v>1980</v>
       </c>
@@ -2300,10 +2582,10 @@
         <v>12</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B11" s="6">
         <v>2015</v>
       </c>
@@ -2317,7 +2599,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B12" s="6">
         <v>1</v>
       </c>
@@ -2331,7 +2613,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B13" s="6">
         <v>5555</v>
       </c>
@@ -2345,7 +2627,7 @@
         <v>1335327</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B14" s="6">
         <v>7777777</v>
       </c>
@@ -2359,11 +2641,3155 @@
         <v>90</v>
       </c>
     </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B17" s="48" t="s">
+        <v>142</v>
+      </c>
+      <c r="C17" s="48"/>
+      <c r="D17" s="48"/>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B18" s="49" t="s">
+        <v>143</v>
+      </c>
+      <c r="C18" s="49"/>
+      <c r="D18" s="49"/>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B30" s="48" t="s">
+        <v>105</v>
+      </c>
+      <c r="C30" s="48"/>
+      <c r="D30" s="48"/>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B31" s="49" t="s">
+        <v>109</v>
+      </c>
+      <c r="C31" s="49"/>
+      <c r="D31" s="49"/>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B33" s="50" t="s">
+        <v>91</v>
+      </c>
+      <c r="C33" s="50"/>
+      <c r="D33" s="50"/>
+      <c r="E33" s="50"/>
+      <c r="F33" s="50"/>
+      <c r="G33" s="50"/>
+      <c r="H33" s="50"/>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B34" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="C34" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="D34" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="E34" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="F34" s="25" t="s">
+        <v>107</v>
+      </c>
+      <c r="G34" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="H34" s="24" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B35" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="C35" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="D35" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="E35" s="26" t="s">
+        <v>110</v>
+      </c>
+      <c r="F35" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="G35" s="26" t="s">
+        <v>112</v>
+      </c>
+      <c r="H35" s="26" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B36" s="6">
+        <v>1980</v>
+      </c>
+      <c r="C36" s="6">
+        <v>7</v>
+      </c>
+      <c r="D36" s="6">
+        <v>12</v>
+      </c>
+      <c r="E36" s="6">
+        <v>12</v>
+      </c>
+      <c r="F36" s="6">
+        <v>59</v>
+      </c>
+      <c r="G36" s="6">
+        <v>58</v>
+      </c>
+      <c r="H36" s="11" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B37" s="6">
+        <v>2015</v>
+      </c>
+      <c r="C37" s="6">
+        <v>4</v>
+      </c>
+      <c r="D37" s="6">
+        <v>30</v>
+      </c>
+      <c r="E37" s="6">
+        <v>1</v>
+      </c>
+      <c r="F37" s="6">
+        <v>30</v>
+      </c>
+      <c r="G37" s="6">
+        <v>30</v>
+      </c>
+      <c r="H37" s="11" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B38" s="6">
+        <v>1</v>
+      </c>
+      <c r="C38" s="6">
+        <v>1</v>
+      </c>
+      <c r="D38" s="6">
+        <v>1</v>
+      </c>
+      <c r="E38" s="6">
+        <v>4</v>
+      </c>
+      <c r="F38" s="6">
+        <v>1</v>
+      </c>
+      <c r="G38" s="6">
+        <v>1</v>
+      </c>
+      <c r="H38" s="11" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B39" s="6">
+        <v>5555</v>
+      </c>
+      <c r="C39" s="6">
+        <v>12</v>
+      </c>
+      <c r="D39" s="6">
+        <v>31</v>
+      </c>
+      <c r="E39" s="6">
+        <v>5</v>
+      </c>
+      <c r="F39" s="6">
+        <v>14</v>
+      </c>
+      <c r="G39" s="6">
+        <v>14</v>
+      </c>
+      <c r="H39" s="11" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B40" s="6">
+        <v>7777777</v>
+      </c>
+      <c r="C40" s="6">
+        <v>7</v>
+      </c>
+      <c r="D40" s="6">
+        <v>7</v>
+      </c>
+      <c r="E40" s="6">
+        <v>22</v>
+      </c>
+      <c r="F40" s="6">
+        <v>7</v>
+      </c>
+      <c r="G40" s="6">
+        <v>7</v>
+      </c>
+      <c r="H40" s="11" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B41" s="6">
+        <v>-1</v>
+      </c>
+      <c r="C41" s="6">
+        <v>10</v>
+      </c>
+      <c r="D41" s="6">
+        <v>10</v>
+      </c>
+      <c r="E41" s="6">
+        <v>3</v>
+      </c>
+      <c r="F41" s="6">
+        <v>20</v>
+      </c>
+      <c r="G41" s="6">
+        <v>1</v>
+      </c>
+      <c r="H41" s="11"/>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B42" s="6">
+        <v>0</v>
+      </c>
+      <c r="C42" s="6">
+        <v>10</v>
+      </c>
+      <c r="D42" s="6">
+        <v>10</v>
+      </c>
+      <c r="E42" s="6">
+        <v>3</v>
+      </c>
+      <c r="F42" s="6">
+        <v>34</v>
+      </c>
+      <c r="G42" s="6">
+        <v>1</v>
+      </c>
+      <c r="H42" s="11"/>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B43" s="6">
+        <v>1876</v>
+      </c>
+      <c r="C43" s="6">
+        <v>-1</v>
+      </c>
+      <c r="D43" s="6">
+        <v>10</v>
+      </c>
+      <c r="E43" s="6">
+        <v>10</v>
+      </c>
+      <c r="F43" s="6">
+        <v>10</v>
+      </c>
+      <c r="G43" s="6">
+        <v>1</v>
+      </c>
+      <c r="H43" s="11"/>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B44" s="6">
+        <v>1854</v>
+      </c>
+      <c r="C44" s="6">
+        <v>0</v>
+      </c>
+      <c r="D44" s="6">
+        <v>10</v>
+      </c>
+      <c r="E44" s="6">
+        <v>10</v>
+      </c>
+      <c r="F44" s="6">
+        <v>10</v>
+      </c>
+      <c r="G44" s="6">
+        <v>1</v>
+      </c>
+      <c r="H44" s="11"/>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B45" s="6">
+        <v>1865</v>
+      </c>
+      <c r="C45" s="6">
+        <v>13</v>
+      </c>
+      <c r="D45" s="6">
+        <v>10</v>
+      </c>
+      <c r="E45" s="6">
+        <v>10</v>
+      </c>
+      <c r="F45" s="6">
+        <v>10</v>
+      </c>
+      <c r="G45" s="6">
+        <v>1</v>
+      </c>
+      <c r="H45" s="11"/>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B46" s="6">
+        <v>1987</v>
+      </c>
+      <c r="C46" s="6">
+        <v>5</v>
+      </c>
+      <c r="D46" s="6">
+        <v>-2</v>
+      </c>
+      <c r="E46" s="6">
+        <v>1</v>
+      </c>
+      <c r="F46" s="6">
+        <v>1</v>
+      </c>
+      <c r="G46" s="6">
+        <v>1</v>
+      </c>
+      <c r="H46" s="11"/>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B47" s="6">
+        <v>1987</v>
+      </c>
+      <c r="C47" s="6">
+        <v>5</v>
+      </c>
+      <c r="D47" s="6">
+        <v>0</v>
+      </c>
+      <c r="E47" s="6">
+        <v>1</v>
+      </c>
+      <c r="F47" s="6">
+        <v>1</v>
+      </c>
+      <c r="G47" s="6">
+        <v>1</v>
+      </c>
+      <c r="H47" s="11"/>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B48" s="6">
+        <v>1987</v>
+      </c>
+      <c r="C48" s="6">
+        <v>5</v>
+      </c>
+      <c r="D48" s="6">
+        <v>32</v>
+      </c>
+      <c r="E48" s="6">
+        <v>1</v>
+      </c>
+      <c r="F48" s="6">
+        <v>1</v>
+      </c>
+      <c r="G48" s="6">
+        <v>1</v>
+      </c>
+      <c r="H48" s="11"/>
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B49" s="6">
+        <v>1987</v>
+      </c>
+      <c r="C49" s="6">
+        <v>6</v>
+      </c>
+      <c r="D49" s="6">
+        <v>6</v>
+      </c>
+      <c r="E49" s="6">
+        <v>-3</v>
+      </c>
+      <c r="F49" s="6">
+        <v>13</v>
+      </c>
+      <c r="G49" s="6">
+        <v>1</v>
+      </c>
+      <c r="H49" s="11"/>
+    </row>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B50" s="6">
+        <v>1876</v>
+      </c>
+      <c r="C50" s="6">
+        <v>4</v>
+      </c>
+      <c r="D50" s="6">
+        <v>6</v>
+      </c>
+      <c r="E50" s="6">
+        <v>23412341</v>
+      </c>
+      <c r="F50" s="6">
+        <v>23</v>
+      </c>
+      <c r="G50" s="6">
+        <v>1</v>
+      </c>
+      <c r="H50" s="11"/>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B51" s="6">
+        <v>1875</v>
+      </c>
+      <c r="C51" s="6">
+        <v>4</v>
+      </c>
+      <c r="D51" s="6">
+        <v>2</v>
+      </c>
+      <c r="E51" s="6">
+        <v>23</v>
+      </c>
+      <c r="F51" s="6">
+        <v>-1</v>
+      </c>
+      <c r="G51" s="6">
+        <v>1</v>
+      </c>
+      <c r="H51" s="11"/>
+    </row>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B52" s="6">
+        <v>1874</v>
+      </c>
+      <c r="C52" s="6">
+        <v>3</v>
+      </c>
+      <c r="D52" s="6">
+        <v>4</v>
+      </c>
+      <c r="E52" s="6">
+        <v>3</v>
+      </c>
+      <c r="F52" s="6">
+        <v>59</v>
+      </c>
+      <c r="G52" s="6">
+        <v>-1</v>
+      </c>
+      <c r="H52" s="11"/>
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B53" s="6">
+        <v>1987</v>
+      </c>
+      <c r="C53" s="6">
+        <v>3</v>
+      </c>
+      <c r="D53" s="6">
+        <v>4</v>
+      </c>
+      <c r="E53" s="6">
+        <v>3</v>
+      </c>
+      <c r="F53" s="6">
+        <v>12</v>
+      </c>
+      <c r="G53" s="6">
+        <v>60</v>
+      </c>
+      <c r="H53" s="11"/>
+    </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B54" s="28"/>
+      <c r="C54" s="28"/>
+      <c r="D54" s="28"/>
+      <c r="E54" s="28"/>
+      <c r="F54" s="28"/>
+      <c r="G54" s="28"/>
+      <c r="H54" s="21"/>
+    </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B55" s="28"/>
+      <c r="C55" s="28"/>
+      <c r="D55" s="28"/>
+      <c r="E55" s="28"/>
+      <c r="F55" s="28"/>
+      <c r="G55" s="28"/>
+      <c r="H55" s="21"/>
+    </row>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B56" s="28"/>
+      <c r="C56" s="28"/>
+      <c r="D56" s="28"/>
+      <c r="E56" s="28"/>
+      <c r="F56" s="28"/>
+      <c r="G56" s="28"/>
+      <c r="H56" s="21"/>
+    </row>
+    <row r="57" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B57" s="28"/>
+      <c r="C57" s="28"/>
+      <c r="D57" s="28"/>
+      <c r="E57" s="28"/>
+      <c r="F57" s="28"/>
+      <c r="G57" s="28"/>
+      <c r="H57" s="21"/>
+    </row>
+    <row r="58" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B58" s="28"/>
+      <c r="C58" s="28"/>
+      <c r="D58" s="28"/>
+      <c r="E58" s="28"/>
+      <c r="F58" s="28"/>
+      <c r="G58" s="28"/>
+      <c r="H58" s="21"/>
+    </row>
+    <row r="59" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B59" s="28"/>
+      <c r="C59" s="28"/>
+      <c r="D59" s="28"/>
+      <c r="E59" s="28"/>
+      <c r="F59" s="28"/>
+      <c r="G59" s="28"/>
+      <c r="H59" s="21"/>
+    </row>
+    <row r="60" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B60" s="28"/>
+      <c r="C60" s="28"/>
+      <c r="D60" s="28"/>
+      <c r="E60" s="28"/>
+      <c r="F60" s="28"/>
+      <c r="G60" s="28"/>
+      <c r="H60" s="21"/>
+    </row>
+    <row r="61" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B61" s="28"/>
+      <c r="C61" s="28"/>
+      <c r="D61" s="28"/>
+      <c r="E61" s="28"/>
+      <c r="F61" s="28"/>
+      <c r="G61" s="28"/>
+      <c r="H61" s="21"/>
+    </row>
+    <row r="62" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B62" s="28"/>
+      <c r="C62" s="28"/>
+      <c r="D62" s="28"/>
+      <c r="E62" s="28"/>
+      <c r="F62" s="28"/>
+      <c r="G62" s="28"/>
+      <c r="H62" s="21"/>
+    </row>
+    <row r="63" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B63" s="28"/>
+      <c r="C63" s="28"/>
+      <c r="D63" s="28"/>
+      <c r="E63" s="28"/>
+      <c r="F63" s="28"/>
+      <c r="G63" s="28"/>
+      <c r="H63" s="21"/>
+    </row>
+    <row r="64" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B64" s="28"/>
+      <c r="C64" s="28"/>
+      <c r="D64" s="28"/>
+      <c r="E64" s="28"/>
+      <c r="F64" s="28"/>
+      <c r="G64" s="28"/>
+      <c r="H64" s="21"/>
+    </row>
+    <row r="67" spans="2:11" x14ac:dyDescent="0.15">
+      <c r="B67" s="48" t="s">
+        <v>155</v>
+      </c>
+      <c r="C67" s="48"/>
+      <c r="D67" s="48"/>
+    </row>
+    <row r="68" spans="2:11" x14ac:dyDescent="0.15">
+      <c r="B68" s="49" t="s">
+        <v>156</v>
+      </c>
+      <c r="C68" s="49"/>
+      <c r="D68" s="49"/>
+    </row>
+    <row r="70" spans="2:11" x14ac:dyDescent="0.15">
+      <c r="B70" s="50" t="s">
+        <v>91</v>
+      </c>
+      <c r="C70" s="50"/>
+      <c r="D70" s="50"/>
+      <c r="E70" s="50"/>
+      <c r="F70" s="50"/>
+      <c r="G70" s="50"/>
+      <c r="H70" s="50"/>
+    </row>
+    <row r="71" spans="2:11" x14ac:dyDescent="0.15">
+      <c r="B71" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="C71" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="D71" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="E71" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="F71" s="25" t="s">
+        <v>107</v>
+      </c>
+      <c r="G71" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="H71" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="I71" s="24" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="2:11" x14ac:dyDescent="0.15">
+      <c r="B72" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="C72" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="D72" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="E72" s="26" t="s">
+        <v>110</v>
+      </c>
+      <c r="F72" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="G72" s="26" t="s">
+        <v>112</v>
+      </c>
+      <c r="H72" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="I72" s="26" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="2:11" x14ac:dyDescent="0.15">
+      <c r="B73" s="6">
+        <v>1980</v>
+      </c>
+      <c r="C73" s="6">
+        <v>7</v>
+      </c>
+      <c r="D73" s="6">
+        <v>12</v>
+      </c>
+      <c r="E73" s="6">
+        <v>12</v>
+      </c>
+      <c r="F73" s="6">
+        <v>59</v>
+      </c>
+      <c r="G73" s="6">
+        <v>58</v>
+      </c>
+      <c r="H73" s="6">
+        <v>4</v>
+      </c>
+      <c r="I73" s="11" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="74" spans="2:11" x14ac:dyDescent="0.15">
+      <c r="B74" s="6">
+        <v>2015</v>
+      </c>
+      <c r="C74" s="6">
+        <v>4</v>
+      </c>
+      <c r="D74" s="6">
+        <v>30</v>
+      </c>
+      <c r="E74" s="6">
+        <v>1</v>
+      </c>
+      <c r="F74" s="6">
+        <v>30</v>
+      </c>
+      <c r="G74" s="6">
+        <v>30</v>
+      </c>
+      <c r="H74" s="6">
+        <v>0</v>
+      </c>
+      <c r="I74" s="11" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="75" spans="2:11" x14ac:dyDescent="0.15">
+      <c r="B75" s="6">
+        <v>1</v>
+      </c>
+      <c r="C75" s="6">
+        <v>1</v>
+      </c>
+      <c r="D75" s="6">
+        <v>1</v>
+      </c>
+      <c r="E75" s="6">
+        <v>4</v>
+      </c>
+      <c r="F75" s="6">
+        <v>1</v>
+      </c>
+      <c r="G75" s="6">
+        <v>1</v>
+      </c>
+      <c r="H75" s="6">
+        <v>999</v>
+      </c>
+      <c r="I75" s="11" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="76" spans="2:11" x14ac:dyDescent="0.15">
+      <c r="B76" s="6">
+        <v>5555</v>
+      </c>
+      <c r="C76" s="6">
+        <v>12</v>
+      </c>
+      <c r="D76" s="6">
+        <v>31</v>
+      </c>
+      <c r="E76" s="6">
+        <v>5</v>
+      </c>
+      <c r="F76" s="6">
+        <v>14</v>
+      </c>
+      <c r="G76" s="6">
+        <v>14</v>
+      </c>
+      <c r="H76" s="6">
+        <v>991</v>
+      </c>
+      <c r="I76" s="11" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="77" spans="2:11" x14ac:dyDescent="0.15">
+      <c r="B77" s="6">
+        <v>7777777</v>
+      </c>
+      <c r="C77" s="6">
+        <v>7</v>
+      </c>
+      <c r="D77" s="6">
+        <v>7</v>
+      </c>
+      <c r="E77" s="6">
+        <v>22</v>
+      </c>
+      <c r="F77" s="6">
+        <v>7</v>
+      </c>
+      <c r="G77" s="6">
+        <v>7</v>
+      </c>
+      <c r="H77" s="6">
+        <v>992</v>
+      </c>
+      <c r="I77" s="11" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="78" spans="2:11" x14ac:dyDescent="0.15">
+      <c r="B78" s="6">
+        <v>-1</v>
+      </c>
+      <c r="C78" s="6">
+        <v>10</v>
+      </c>
+      <c r="D78" s="6">
+        <v>10</v>
+      </c>
+      <c r="E78" s="6">
+        <v>3</v>
+      </c>
+      <c r="F78" s="6">
+        <v>20</v>
+      </c>
+      <c r="G78" s="6">
+        <v>1</v>
+      </c>
+      <c r="H78" s="29">
+        <v>1</v>
+      </c>
+      <c r="I78" s="11"/>
+      <c r="K78" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="79" spans="2:11" x14ac:dyDescent="0.15">
+      <c r="B79" s="6">
+        <v>0</v>
+      </c>
+      <c r="C79" s="6">
+        <v>10</v>
+      </c>
+      <c r="D79" s="6">
+        <v>10</v>
+      </c>
+      <c r="E79" s="6">
+        <v>3</v>
+      </c>
+      <c r="F79" s="6">
+        <v>34</v>
+      </c>
+      <c r="G79" s="6">
+        <v>1</v>
+      </c>
+      <c r="H79" s="29">
+        <v>1</v>
+      </c>
+      <c r="I79" s="11"/>
+      <c r="K79" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="80" spans="2:11" x14ac:dyDescent="0.15">
+      <c r="B80" s="6">
+        <v>1876</v>
+      </c>
+      <c r="C80" s="6">
+        <v>-1</v>
+      </c>
+      <c r="D80" s="6">
+        <v>10</v>
+      </c>
+      <c r="E80" s="6">
+        <v>10</v>
+      </c>
+      <c r="F80" s="6">
+        <v>10</v>
+      </c>
+      <c r="G80" s="6">
+        <v>1</v>
+      </c>
+      <c r="H80" s="29">
+        <v>1</v>
+      </c>
+      <c r="I80" s="11"/>
+      <c r="K80" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="81" spans="2:11" x14ac:dyDescent="0.15">
+      <c r="B81" s="6">
+        <v>1854</v>
+      </c>
+      <c r="C81" s="6">
+        <v>0</v>
+      </c>
+      <c r="D81" s="6">
+        <v>10</v>
+      </c>
+      <c r="E81" s="6">
+        <v>10</v>
+      </c>
+      <c r="F81" s="6">
+        <v>10</v>
+      </c>
+      <c r="G81" s="6">
+        <v>1</v>
+      </c>
+      <c r="H81" s="29">
+        <v>1</v>
+      </c>
+      <c r="I81" s="11"/>
+      <c r="K81" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="82" spans="2:11" x14ac:dyDescent="0.15">
+      <c r="B82" s="6">
+        <v>1865</v>
+      </c>
+      <c r="C82" s="6">
+        <v>13</v>
+      </c>
+      <c r="D82" s="6">
+        <v>10</v>
+      </c>
+      <c r="E82" s="6">
+        <v>10</v>
+      </c>
+      <c r="F82" s="6">
+        <v>10</v>
+      </c>
+      <c r="G82" s="6">
+        <v>1</v>
+      </c>
+      <c r="H82" s="29">
+        <v>1</v>
+      </c>
+      <c r="I82" s="11"/>
+      <c r="K82" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="83" spans="2:11" x14ac:dyDescent="0.15">
+      <c r="B83" s="6">
+        <v>1987</v>
+      </c>
+      <c r="C83" s="6">
+        <v>5</v>
+      </c>
+      <c r="D83" s="6">
+        <v>-2</v>
+      </c>
+      <c r="E83" s="6">
+        <v>1</v>
+      </c>
+      <c r="F83" s="6">
+        <v>1</v>
+      </c>
+      <c r="G83" s="6">
+        <v>1</v>
+      </c>
+      <c r="H83" s="29">
+        <v>1</v>
+      </c>
+      <c r="I83" s="11"/>
+      <c r="K83" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="84" spans="2:11" x14ac:dyDescent="0.15">
+      <c r="B84" s="6">
+        <v>1987</v>
+      </c>
+      <c r="C84" s="6">
+        <v>5</v>
+      </c>
+      <c r="D84" s="6">
+        <v>0</v>
+      </c>
+      <c r="E84" s="6">
+        <v>1</v>
+      </c>
+      <c r="F84" s="6">
+        <v>1</v>
+      </c>
+      <c r="G84" s="6">
+        <v>1</v>
+      </c>
+      <c r="H84" s="29">
+        <v>1</v>
+      </c>
+      <c r="I84" s="11"/>
+      <c r="K84" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="85" spans="2:11" x14ac:dyDescent="0.15">
+      <c r="B85" s="6">
+        <v>1987</v>
+      </c>
+      <c r="C85" s="6">
+        <v>5</v>
+      </c>
+      <c r="D85" s="6">
+        <v>32</v>
+      </c>
+      <c r="E85" s="6">
+        <v>1</v>
+      </c>
+      <c r="F85" s="6">
+        <v>1</v>
+      </c>
+      <c r="G85" s="6">
+        <v>1</v>
+      </c>
+      <c r="H85" s="29">
+        <v>1</v>
+      </c>
+      <c r="I85" s="11"/>
+      <c r="K85" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="86" spans="2:11" x14ac:dyDescent="0.15">
+      <c r="B86" s="6">
+        <v>1987</v>
+      </c>
+      <c r="C86" s="6">
+        <v>6</v>
+      </c>
+      <c r="D86" s="6">
+        <v>6</v>
+      </c>
+      <c r="E86" s="6">
+        <v>-3</v>
+      </c>
+      <c r="F86" s="6">
+        <v>13</v>
+      </c>
+      <c r="G86" s="6">
+        <v>1</v>
+      </c>
+      <c r="H86" s="29">
+        <v>1</v>
+      </c>
+      <c r="I86" s="11"/>
+      <c r="K86" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="87" spans="2:11" x14ac:dyDescent="0.15">
+      <c r="B87" s="6">
+        <v>1876</v>
+      </c>
+      <c r="C87" s="6">
+        <v>4</v>
+      </c>
+      <c r="D87" s="6">
+        <v>6</v>
+      </c>
+      <c r="E87" s="6">
+        <v>23412341</v>
+      </c>
+      <c r="F87" s="6">
+        <v>23</v>
+      </c>
+      <c r="G87" s="6">
+        <v>1</v>
+      </c>
+      <c r="H87" s="29">
+        <v>1</v>
+      </c>
+      <c r="I87" s="11"/>
+      <c r="K87" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="88" spans="2:11" x14ac:dyDescent="0.15">
+      <c r="B88" s="6">
+        <v>1875</v>
+      </c>
+      <c r="C88" s="6">
+        <v>4</v>
+      </c>
+      <c r="D88" s="6">
+        <v>2</v>
+      </c>
+      <c r="E88" s="6">
+        <v>23</v>
+      </c>
+      <c r="F88" s="6">
+        <v>-1</v>
+      </c>
+      <c r="G88" s="6">
+        <v>1</v>
+      </c>
+      <c r="H88" s="29">
+        <v>1</v>
+      </c>
+      <c r="I88" s="11"/>
+      <c r="K88" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="89" spans="2:11" x14ac:dyDescent="0.15">
+      <c r="B89" s="6">
+        <v>1874</v>
+      </c>
+      <c r="C89" s="6">
+        <v>3</v>
+      </c>
+      <c r="D89" s="6">
+        <v>4</v>
+      </c>
+      <c r="E89" s="6">
+        <v>3</v>
+      </c>
+      <c r="F89" s="6">
+        <v>59</v>
+      </c>
+      <c r="G89" s="6">
+        <v>-1</v>
+      </c>
+      <c r="H89" s="29">
+        <v>1</v>
+      </c>
+      <c r="I89" s="11"/>
+      <c r="K89" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="90" spans="2:11" x14ac:dyDescent="0.15">
+      <c r="B90" s="6">
+        <v>1987</v>
+      </c>
+      <c r="C90" s="6">
+        <v>3</v>
+      </c>
+      <c r="D90" s="6">
+        <v>4</v>
+      </c>
+      <c r="E90" s="6">
+        <v>3</v>
+      </c>
+      <c r="F90" s="6">
+        <v>12</v>
+      </c>
+      <c r="G90" s="6">
+        <v>60</v>
+      </c>
+      <c r="H90" s="29">
+        <v>1</v>
+      </c>
+      <c r="I90" s="11"/>
+      <c r="K90" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="91" spans="2:11" x14ac:dyDescent="0.15">
+      <c r="B91" s="6">
+        <v>1987</v>
+      </c>
+      <c r="C91" s="6">
+        <v>3</v>
+      </c>
+      <c r="D91" s="6">
+        <v>4</v>
+      </c>
+      <c r="E91" s="6">
+        <v>3</v>
+      </c>
+      <c r="F91" s="6">
+        <v>12</v>
+      </c>
+      <c r="G91" s="6">
+        <v>1</v>
+      </c>
+      <c r="H91" s="29">
+        <v>-1</v>
+      </c>
+      <c r="I91" s="11"/>
+      <c r="K91" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="92" spans="2:11" x14ac:dyDescent="0.15">
+      <c r="B92" s="6">
+        <v>1987</v>
+      </c>
+      <c r="C92" s="6">
+        <v>3</v>
+      </c>
+      <c r="D92" s="6">
+        <v>4</v>
+      </c>
+      <c r="E92" s="6">
+        <v>3</v>
+      </c>
+      <c r="F92" s="6">
+        <v>12</v>
+      </c>
+      <c r="G92" s="6">
+        <v>1</v>
+      </c>
+      <c r="H92" s="29">
+        <v>1000</v>
+      </c>
+      <c r="I92" s="11"/>
+      <c r="K92" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="93" spans="2:11" x14ac:dyDescent="0.15">
+      <c r="B93" s="28"/>
+      <c r="C93" s="28"/>
+      <c r="D93" s="28"/>
+      <c r="E93" s="28"/>
+      <c r="F93" s="28"/>
+      <c r="G93" s="28"/>
+      <c r="H93" s="28"/>
+      <c r="I93" s="21"/>
+    </row>
+    <row r="94" spans="2:11" x14ac:dyDescent="0.15">
+      <c r="B94" s="28"/>
+      <c r="C94" s="28"/>
+      <c r="D94" s="28"/>
+      <c r="E94" s="28"/>
+      <c r="F94" s="28"/>
+      <c r="G94" s="28"/>
+      <c r="H94" s="28"/>
+      <c r="I94" s="21"/>
+    </row>
+    <row r="95" spans="2:11" x14ac:dyDescent="0.15">
+      <c r="B95" s="28"/>
+      <c r="C95" s="28"/>
+      <c r="D95" s="28"/>
+      <c r="E95" s="28"/>
+      <c r="F95" s="28"/>
+      <c r="G95" s="28"/>
+      <c r="H95" s="28"/>
+      <c r="I95" s="21"/>
+    </row>
+    <row r="96" spans="2:11" x14ac:dyDescent="0.15">
+      <c r="B96" s="28"/>
+      <c r="C96" s="28"/>
+      <c r="D96" s="28"/>
+      <c r="E96" s="28"/>
+      <c r="F96" s="28"/>
+      <c r="G96" s="28"/>
+      <c r="H96" s="28"/>
+      <c r="I96" s="21"/>
+    </row>
+    <row r="97" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B97" s="28"/>
+      <c r="C97" s="28"/>
+      <c r="D97" s="28"/>
+      <c r="E97" s="28"/>
+      <c r="F97" s="28"/>
+      <c r="G97" s="28"/>
+      <c r="H97" s="28"/>
+      <c r="I97" s="21"/>
+    </row>
+    <row r="98" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B98" s="28"/>
+      <c r="C98" s="28"/>
+      <c r="D98" s="28"/>
+      <c r="E98" s="28"/>
+      <c r="F98" s="28"/>
+      <c r="G98" s="28"/>
+      <c r="H98" s="28"/>
+      <c r="I98" s="21"/>
+    </row>
+    <row r="99" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B99" s="28"/>
+      <c r="C99" s="28"/>
+      <c r="D99" s="28"/>
+      <c r="E99" s="28"/>
+      <c r="F99" s="28"/>
+      <c r="G99" s="28"/>
+      <c r="H99" s="28"/>
+      <c r="I99" s="21"/>
+    </row>
+    <row r="100" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B100" s="28"/>
+      <c r="C100" s="28"/>
+      <c r="D100" s="28"/>
+      <c r="E100" s="28"/>
+      <c r="F100" s="28"/>
+      <c r="G100" s="28"/>
+      <c r="H100" s="28"/>
+      <c r="I100" s="21"/>
+    </row>
+    <row r="101" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B101" s="28"/>
+      <c r="C101" s="28"/>
+      <c r="D101" s="28"/>
+      <c r="E101" s="28"/>
+      <c r="F101" s="28"/>
+      <c r="G101" s="28"/>
+      <c r="H101" s="28"/>
+      <c r="I101" s="21"/>
+    </row>
+    <row r="102" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B102" s="28"/>
+      <c r="C102" s="28"/>
+      <c r="D102" s="28"/>
+      <c r="E102" s="28"/>
+      <c r="F102" s="28"/>
+      <c r="G102" s="28"/>
+      <c r="H102" s="28"/>
+      <c r="I102" s="21"/>
+    </row>
+    <row r="103" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B103" s="28"/>
+      <c r="C103" s="28"/>
+      <c r="D103" s="28"/>
+      <c r="E103" s="28"/>
+      <c r="F103" s="28"/>
+      <c r="G103" s="28"/>
+      <c r="H103" s="28"/>
+      <c r="I103" s="21"/>
+    </row>
+    <row r="104" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B104" s="28"/>
+      <c r="C104" s="28"/>
+      <c r="D104" s="28"/>
+      <c r="E104" s="28"/>
+      <c r="F104" s="28"/>
+      <c r="G104" s="28"/>
+      <c r="H104" s="28"/>
+      <c r="I104" s="21"/>
+    </row>
+    <row r="105" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B105" s="28"/>
+      <c r="C105" s="28"/>
+      <c r="D105" s="28"/>
+      <c r="E105" s="28"/>
+      <c r="F105" s="28"/>
+      <c r="G105" s="28"/>
+      <c r="H105" s="28"/>
+      <c r="I105" s="21"/>
+    </row>
+    <row r="107" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B107" s="50" t="s">
+        <v>91</v>
+      </c>
+      <c r="C107" s="50" t="s">
+        <v>91</v>
+      </c>
+      <c r="D107" s="50" t="s">
+        <v>91</v>
+      </c>
+      <c r="E107" s="50" t="s">
+        <v>91</v>
+      </c>
+      <c r="F107" s="50" t="s">
+        <v>91</v>
+      </c>
+      <c r="G107" s="50" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="108" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B108" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="C108" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="D108" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="E108" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="F108" s="25" t="s">
+        <v>107</v>
+      </c>
+      <c r="G108" s="24" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B109" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="C109" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="D109" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="E109" s="26" t="s">
+        <v>110</v>
+      </c>
+      <c r="F109" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="G109" s="26" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B110" s="6">
+        <v>1980</v>
+      </c>
+      <c r="C110" s="6">
+        <v>7</v>
+      </c>
+      <c r="D110" s="6">
+        <v>12</v>
+      </c>
+      <c r="E110" s="6">
+        <v>12</v>
+      </c>
+      <c r="F110" s="6">
+        <v>59</v>
+      </c>
+      <c r="G110" s="11" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="111" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B111" s="6">
+        <v>2015</v>
+      </c>
+      <c r="C111" s="6">
+        <v>4</v>
+      </c>
+      <c r="D111" s="6">
+        <v>30</v>
+      </c>
+      <c r="E111" s="6">
+        <v>1</v>
+      </c>
+      <c r="F111" s="6">
+        <v>30</v>
+      </c>
+      <c r="G111" s="11" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="112" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B112" s="6">
+        <v>1</v>
+      </c>
+      <c r="C112" s="6">
+        <v>1</v>
+      </c>
+      <c r="D112" s="6">
+        <v>1</v>
+      </c>
+      <c r="E112" s="6">
+        <v>4</v>
+      </c>
+      <c r="F112" s="6">
+        <v>1</v>
+      </c>
+      <c r="G112" s="11" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="113" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B113" s="6">
+        <v>5555</v>
+      </c>
+      <c r="C113" s="6">
+        <v>12</v>
+      </c>
+      <c r="D113" s="6">
+        <v>31</v>
+      </c>
+      <c r="E113" s="6">
+        <v>5</v>
+      </c>
+      <c r="F113" s="6">
+        <v>14</v>
+      </c>
+      <c r="G113" s="11" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="114" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B114" s="6">
+        <v>7777777</v>
+      </c>
+      <c r="C114" s="6">
+        <v>7</v>
+      </c>
+      <c r="D114" s="6">
+        <v>7</v>
+      </c>
+      <c r="E114" s="6">
+        <v>22</v>
+      </c>
+      <c r="F114" s="6">
+        <v>7</v>
+      </c>
+      <c r="G114" s="11" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="115" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B115" s="6">
+        <v>-1</v>
+      </c>
+      <c r="C115" s="6">
+        <v>10</v>
+      </c>
+      <c r="D115" s="6">
+        <v>10</v>
+      </c>
+      <c r="E115" s="6">
+        <v>3</v>
+      </c>
+      <c r="F115" s="6">
+        <v>20</v>
+      </c>
+      <c r="G115" s="11"/>
+      <c r="I115" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="116" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B116" s="6">
+        <v>0</v>
+      </c>
+      <c r="C116" s="6">
+        <v>10</v>
+      </c>
+      <c r="D116" s="6">
+        <v>10</v>
+      </c>
+      <c r="E116" s="6">
+        <v>3</v>
+      </c>
+      <c r="F116" s="6">
+        <v>34</v>
+      </c>
+      <c r="G116" s="11"/>
+      <c r="I116" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="117" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B117" s="6">
+        <v>1876</v>
+      </c>
+      <c r="C117" s="6">
+        <v>-1</v>
+      </c>
+      <c r="D117" s="6">
+        <v>10</v>
+      </c>
+      <c r="E117" s="6">
+        <v>10</v>
+      </c>
+      <c r="F117" s="6">
+        <v>10</v>
+      </c>
+      <c r="G117" s="11"/>
+      <c r="I117" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="118" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B118" s="6">
+        <v>1854</v>
+      </c>
+      <c r="C118" s="6">
+        <v>0</v>
+      </c>
+      <c r="D118" s="6">
+        <v>10</v>
+      </c>
+      <c r="E118" s="6">
+        <v>10</v>
+      </c>
+      <c r="F118" s="6">
+        <v>10</v>
+      </c>
+      <c r="G118" s="11"/>
+      <c r="I118" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="119" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B119" s="6">
+        <v>1865</v>
+      </c>
+      <c r="C119" s="6">
+        <v>13</v>
+      </c>
+      <c r="D119" s="6">
+        <v>10</v>
+      </c>
+      <c r="E119" s="6">
+        <v>10</v>
+      </c>
+      <c r="F119" s="6">
+        <v>10</v>
+      </c>
+      <c r="G119" s="27"/>
+      <c r="I119" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="120" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B120" s="6">
+        <v>1987</v>
+      </c>
+      <c r="C120" s="6">
+        <v>5</v>
+      </c>
+      <c r="D120" s="6">
+        <v>-2</v>
+      </c>
+      <c r="E120" s="6">
+        <v>1</v>
+      </c>
+      <c r="F120" s="6">
+        <v>1</v>
+      </c>
+      <c r="G120" s="27"/>
+      <c r="I120" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="121" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B121" s="6">
+        <v>1987</v>
+      </c>
+      <c r="C121" s="6">
+        <v>5</v>
+      </c>
+      <c r="D121" s="6">
+        <v>0</v>
+      </c>
+      <c r="E121" s="6">
+        <v>1</v>
+      </c>
+      <c r="F121" s="6">
+        <v>1</v>
+      </c>
+      <c r="G121" s="27"/>
+      <c r="I121" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="122" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B122" s="6">
+        <v>1987</v>
+      </c>
+      <c r="C122" s="6">
+        <v>5</v>
+      </c>
+      <c r="D122" s="6">
+        <v>32</v>
+      </c>
+      <c r="E122" s="6">
+        <v>1</v>
+      </c>
+      <c r="F122" s="6">
+        <v>1</v>
+      </c>
+      <c r="G122" s="27"/>
+      <c r="I122" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="123" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B123" s="6">
+        <v>1987</v>
+      </c>
+      <c r="C123" s="6">
+        <v>6</v>
+      </c>
+      <c r="D123" s="6">
+        <v>6</v>
+      </c>
+      <c r="E123" s="6">
+        <v>-3</v>
+      </c>
+      <c r="F123" s="6">
+        <v>13</v>
+      </c>
+      <c r="G123" s="27"/>
+      <c r="I123" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="124" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B124" s="6">
+        <v>1876</v>
+      </c>
+      <c r="C124" s="6">
+        <v>4</v>
+      </c>
+      <c r="D124" s="6">
+        <v>6</v>
+      </c>
+      <c r="E124" s="6">
+        <v>23412341</v>
+      </c>
+      <c r="F124" s="6">
+        <v>23</v>
+      </c>
+      <c r="G124" s="27"/>
+      <c r="I124" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="125" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B125" s="6">
+        <v>1875</v>
+      </c>
+      <c r="C125" s="6">
+        <v>4</v>
+      </c>
+      <c r="D125" s="6">
+        <v>2</v>
+      </c>
+      <c r="E125" s="6">
+        <v>23</v>
+      </c>
+      <c r="F125" s="6">
+        <v>-1</v>
+      </c>
+      <c r="G125" s="27"/>
+      <c r="I125" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="126" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B126" s="6">
+        <v>1874</v>
+      </c>
+      <c r="C126" s="6">
+        <v>3</v>
+      </c>
+      <c r="D126" s="6">
+        <v>4</v>
+      </c>
+      <c r="E126" s="6">
+        <v>3</v>
+      </c>
+      <c r="F126" s="6">
+        <v>61</v>
+      </c>
+      <c r="G126" s="27"/>
+      <c r="I126" t="s">
+        <v>172</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="12">
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B107:G107"/>
+    <mergeCell ref="B67:D67"/>
+    <mergeCell ref="B68:D68"/>
+    <mergeCell ref="B70:H70"/>
+    <mergeCell ref="B33:H33"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ECBA2BC-33CC-4577-BDBD-94A2E6F0BB52}">
+  <dimension ref="B4:I123"/>
+  <sheetViews>
+    <sheetView topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="I79" sqref="I79"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="2" max="2" width="23.33203125" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" customWidth="1"/>
+    <col min="4" max="4" width="40.1640625" customWidth="1"/>
+    <col min="5" max="5" width="19.83203125" customWidth="1"/>
+    <col min="6" max="6" width="23.83203125" customWidth="1"/>
+    <col min="7" max="7" width="28.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B4" s="48" t="s">
+        <v>120</v>
+      </c>
+      <c r="C4" s="48"/>
+      <c r="D4" s="48"/>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B5" s="49" t="s">
+        <v>115</v>
+      </c>
+      <c r="C5" s="49"/>
+      <c r="D5" s="49"/>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B8" s="51" t="s">
+        <v>121</v>
+      </c>
+      <c r="C8" s="52"/>
+      <c r="D8" s="52"/>
+      <c r="E8" s="52"/>
+      <c r="F8" s="52"/>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B10" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B11" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="C11" s="6">
+        <v>2</v>
+      </c>
+      <c r="D11" s="6">
+        <v>3</v>
+      </c>
+      <c r="E11" s="6">
+        <v>4</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B12" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="C12" s="6">
+        <v>0</v>
+      </c>
+      <c r="D12" s="6">
+        <v>0</v>
+      </c>
+      <c r="E12" s="6">
+        <v>0</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B13" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="C13" s="6">
+        <v>23</v>
+      </c>
+      <c r="D13" s="6">
+        <v>59</v>
+      </c>
+      <c r="E13" s="6">
+        <v>59</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B14" s="40">
+        <v>44720</v>
+      </c>
+      <c r="C14" s="29"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="41">
+        <v>44720</v>
+      </c>
+      <c r="I14" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B15" s="40"/>
+      <c r="C15" s="6">
+        <v>0</v>
+      </c>
+      <c r="D15" s="6">
+        <v>0</v>
+      </c>
+      <c r="E15" s="6">
+        <v>0</v>
+      </c>
+      <c r="F15" s="11"/>
+      <c r="I15" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B16" s="40">
+        <v>44720</v>
+      </c>
+      <c r="C16" s="6">
+        <v>24</v>
+      </c>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="11"/>
+      <c r="I16" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B17" s="40">
+        <v>44720</v>
+      </c>
+      <c r="C17" s="6">
+        <v>-1</v>
+      </c>
+      <c r="D17" s="6">
+        <v>1</v>
+      </c>
+      <c r="E17" s="6"/>
+      <c r="F17" s="11"/>
+      <c r="I17" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B18" s="40">
+        <v>44720</v>
+      </c>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6">
+        <v>60</v>
+      </c>
+      <c r="E18" s="6"/>
+      <c r="F18" s="11"/>
+      <c r="I18" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B19" s="40">
+        <v>44720</v>
+      </c>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6">
+        <v>-1</v>
+      </c>
+      <c r="E19" s="6"/>
+      <c r="F19" s="11"/>
+      <c r="I19" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B20" s="40">
+        <v>44720</v>
+      </c>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6">
+        <v>60</v>
+      </c>
+      <c r="F20" s="11"/>
+      <c r="I20" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B21" s="40">
+        <v>44720</v>
+      </c>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6">
+        <v>-1</v>
+      </c>
+      <c r="F21" s="11"/>
+      <c r="I21" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B27" s="48" t="s">
+        <v>168</v>
+      </c>
+      <c r="C27" s="48"/>
+      <c r="D27" s="48"/>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B28" s="49" t="s">
+        <v>166</v>
+      </c>
+      <c r="C28" s="49"/>
+      <c r="D28" s="49"/>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B31" s="53" t="s">
+        <v>167</v>
+      </c>
+      <c r="C31" s="54"/>
+      <c r="D31" s="54"/>
+      <c r="E31" s="55"/>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B32" s="42" t="s">
+        <v>2</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D32" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B33" s="43" t="s">
+        <v>113</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D33" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="E33" s="44" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B34" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="C34" s="6">
+        <v>2</v>
+      </c>
+      <c r="D34" s="6">
+        <v>3</v>
+      </c>
+      <c r="E34" s="11" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B35" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="C35" s="6">
+        <v>0</v>
+      </c>
+      <c r="D35" s="6">
+        <v>0</v>
+      </c>
+      <c r="E35" s="11" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B36" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="C36" s="6">
+        <v>23</v>
+      </c>
+      <c r="D36" s="6">
+        <v>59</v>
+      </c>
+      <c r="E36" s="11" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B37" s="41">
+        <v>44720</v>
+      </c>
+      <c r="C37" s="29"/>
+      <c r="D37" s="29"/>
+      <c r="E37" s="41">
+        <v>44720</v>
+      </c>
+      <c r="G37" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B38" s="41"/>
+      <c r="C38" s="6">
+        <v>0</v>
+      </c>
+      <c r="D38" s="6">
+        <v>0</v>
+      </c>
+      <c r="E38" s="11"/>
+      <c r="G38" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B39" s="41">
+        <v>44720</v>
+      </c>
+      <c r="C39" s="6">
+        <v>24</v>
+      </c>
+      <c r="D39" s="6"/>
+      <c r="E39" s="11"/>
+      <c r="G39" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B40" s="41">
+        <v>44720</v>
+      </c>
+      <c r="C40" s="6">
+        <v>-1</v>
+      </c>
+      <c r="D40" s="6">
+        <v>1</v>
+      </c>
+      <c r="E40" s="11"/>
+      <c r="G40" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B41" s="41">
+        <v>44720</v>
+      </c>
+      <c r="C41" s="6"/>
+      <c r="D41" s="6">
+        <v>60</v>
+      </c>
+      <c r="E41" s="11"/>
+      <c r="G41" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B42" s="41">
+        <v>44720</v>
+      </c>
+      <c r="C42" s="6"/>
+      <c r="D42" s="6">
+        <v>-1</v>
+      </c>
+      <c r="E42" s="11"/>
+      <c r="G42" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B43" s="41">
+        <v>44720</v>
+      </c>
+      <c r="C43" s="6">
+        <v>24</v>
+      </c>
+      <c r="D43" s="6"/>
+      <c r="E43" s="11"/>
+      <c r="G43" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B47" s="21"/>
+      <c r="C47" s="28"/>
+      <c r="D47" s="28"/>
+      <c r="E47" s="28"/>
+      <c r="F47" s="21"/>
+    </row>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B48" s="21"/>
+      <c r="C48" s="28"/>
+      <c r="D48" s="28"/>
+      <c r="E48" s="28"/>
+      <c r="F48" s="21"/>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="B49" s="21"/>
+      <c r="C49" s="28"/>
+      <c r="D49" s="28"/>
+      <c r="E49" s="28"/>
+      <c r="F49" s="21"/>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="B50" s="21"/>
+      <c r="C50" s="28"/>
+      <c r="D50" s="28"/>
+      <c r="E50" s="28"/>
+      <c r="F50" s="21"/>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="B51" s="21"/>
+      <c r="C51" s="28"/>
+      <c r="D51" s="28"/>
+      <c r="E51" s="28"/>
+      <c r="F51" s="21"/>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="B52" s="21"/>
+      <c r="C52" s="28"/>
+      <c r="D52" s="28"/>
+      <c r="E52" s="28"/>
+      <c r="F52" s="21"/>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="B53" s="21"/>
+      <c r="C53" s="28"/>
+      <c r="D53" s="28"/>
+      <c r="E53" s="28"/>
+      <c r="F53" s="21"/>
+    </row>
+    <row r="54" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="B54" s="21"/>
+      <c r="C54" s="28"/>
+      <c r="D54" s="28"/>
+      <c r="E54" s="28"/>
+      <c r="F54" s="21"/>
+    </row>
+    <row r="55" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="B55" s="21"/>
+      <c r="C55" s="28"/>
+      <c r="D55" s="28"/>
+      <c r="E55" s="28"/>
+      <c r="F55" s="21"/>
+    </row>
+    <row r="56" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="B56" s="21"/>
+      <c r="C56" s="28"/>
+      <c r="D56" s="28"/>
+      <c r="E56" s="28"/>
+      <c r="F56" s="21"/>
+    </row>
+    <row r="57" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="B57" s="21"/>
+      <c r="C57" s="28"/>
+      <c r="D57" s="28"/>
+      <c r="E57" s="28"/>
+      <c r="F57" s="21"/>
+    </row>
+    <row r="61" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="B61" s="48" t="s">
+        <v>122</v>
+      </c>
+      <c r="C61" s="48"/>
+      <c r="D61" s="48"/>
+    </row>
+    <row r="62" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="B62" s="49" t="s">
+        <v>128</v>
+      </c>
+      <c r="C62" s="49"/>
+      <c r="D62" s="49"/>
+    </row>
+    <row r="65" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B65" s="51" t="s">
+        <v>129</v>
+      </c>
+      <c r="C65" s="52"/>
+      <c r="D65" s="52"/>
+      <c r="E65" s="52"/>
+      <c r="F65" s="52"/>
+      <c r="G65" s="52"/>
+    </row>
+    <row r="66" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B66" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D66" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="E66" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="F66" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B67" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D67" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="E67" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="F67" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="G67" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B68" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="C68" s="6">
+        <v>2</v>
+      </c>
+      <c r="D68" s="6">
+        <v>3</v>
+      </c>
+      <c r="E68" s="6">
+        <v>4</v>
+      </c>
+      <c r="F68" s="6">
+        <v>4</v>
+      </c>
+      <c r="G68" s="11" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="69" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B69" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="C69" s="6">
+        <v>0</v>
+      </c>
+      <c r="D69" s="6">
+        <v>0</v>
+      </c>
+      <c r="E69" s="6">
+        <v>0</v>
+      </c>
+      <c r="F69" s="6">
+        <v>0</v>
+      </c>
+      <c r="G69" s="11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="70" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B70" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="C70" s="6">
+        <v>23</v>
+      </c>
+      <c r="D70" s="6">
+        <v>59</v>
+      </c>
+      <c r="E70" s="6">
+        <v>59</v>
+      </c>
+      <c r="F70" s="6">
+        <v>999</v>
+      </c>
+      <c r="G70" s="11" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="71" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B71" s="41">
+        <v>44720</v>
+      </c>
+      <c r="C71" s="29">
+        <v>0</v>
+      </c>
+      <c r="D71" s="29">
+        <v>0</v>
+      </c>
+      <c r="E71" s="29">
+        <v>0</v>
+      </c>
+      <c r="F71" s="29">
+        <v>-1</v>
+      </c>
+      <c r="G71" s="11"/>
+      <c r="I71" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="72" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B72" s="41"/>
+      <c r="C72" s="6">
+        <v>0</v>
+      </c>
+      <c r="D72" s="6">
+        <v>0</v>
+      </c>
+      <c r="E72" s="6">
+        <v>0</v>
+      </c>
+      <c r="F72" s="29">
+        <v>1</v>
+      </c>
+      <c r="G72" s="11"/>
+      <c r="I72" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="73" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B73" s="41">
+        <v>44720</v>
+      </c>
+      <c r="C73" s="6">
+        <v>24</v>
+      </c>
+      <c r="D73" s="6"/>
+      <c r="E73" s="6"/>
+      <c r="F73" s="29">
+        <v>1</v>
+      </c>
+      <c r="G73" s="11"/>
+      <c r="I73" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="74" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B74" s="41">
+        <v>44720</v>
+      </c>
+      <c r="C74" s="6">
+        <v>-1</v>
+      </c>
+      <c r="D74" s="6">
+        <v>1</v>
+      </c>
+      <c r="E74" s="6"/>
+      <c r="F74" s="29">
+        <v>1</v>
+      </c>
+      <c r="G74" s="11"/>
+      <c r="I74" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="75" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B75" s="41">
+        <v>44720</v>
+      </c>
+      <c r="C75" s="6"/>
+      <c r="D75" s="6">
+        <v>60</v>
+      </c>
+      <c r="E75" s="6"/>
+      <c r="F75" s="29">
+        <v>1</v>
+      </c>
+      <c r="G75" s="11"/>
+      <c r="I75" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="76" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B76" s="41">
+        <v>44720</v>
+      </c>
+      <c r="C76" s="6"/>
+      <c r="D76" s="6">
+        <v>-1</v>
+      </c>
+      <c r="E76" s="6"/>
+      <c r="F76" s="29">
+        <v>1</v>
+      </c>
+      <c r="G76" s="11"/>
+      <c r="I76" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="77" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B77" s="41">
+        <v>44720</v>
+      </c>
+      <c r="C77" s="6"/>
+      <c r="D77" s="6"/>
+      <c r="E77" s="6">
+        <v>60</v>
+      </c>
+      <c r="F77" s="29">
+        <v>1</v>
+      </c>
+      <c r="G77" s="11"/>
+      <c r="I77" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="78" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B78" s="41">
+        <v>44720</v>
+      </c>
+      <c r="C78" s="6"/>
+      <c r="D78" s="6"/>
+      <c r="E78" s="6">
+        <v>-1</v>
+      </c>
+      <c r="F78" s="29">
+        <v>1</v>
+      </c>
+      <c r="G78" s="11"/>
+      <c r="I78" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="79" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B79" s="41">
+        <v>44725</v>
+      </c>
+      <c r="C79" s="29">
+        <v>1</v>
+      </c>
+      <c r="D79" s="29">
+        <v>1</v>
+      </c>
+      <c r="E79" s="29">
+        <v>1</v>
+      </c>
+      <c r="F79" s="29">
+        <v>1000</v>
+      </c>
+      <c r="G79" s="11"/>
+      <c r="I79" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="80" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B80" s="21"/>
+      <c r="C80" s="28"/>
+      <c r="D80" s="28"/>
+      <c r="E80" s="28"/>
+      <c r="F80" s="28"/>
+      <c r="G80" s="21"/>
+    </row>
+    <row r="81" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B81" s="21"/>
+      <c r="C81" s="28"/>
+      <c r="D81" s="28"/>
+      <c r="E81" s="28"/>
+      <c r="F81" s="28"/>
+      <c r="G81" s="21"/>
+    </row>
+    <row r="82" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B82" s="21"/>
+      <c r="C82" s="28"/>
+      <c r="D82" s="28"/>
+      <c r="E82" s="28"/>
+      <c r="F82" s="28"/>
+      <c r="G82" s="21"/>
+    </row>
+    <row r="83" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B83" s="21"/>
+      <c r="C83" s="28"/>
+      <c r="D83" s="28"/>
+      <c r="E83" s="28"/>
+      <c r="F83" s="28"/>
+      <c r="G83" s="21"/>
+    </row>
+    <row r="84" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B84" s="21"/>
+      <c r="C84" s="28"/>
+      <c r="D84" s="28"/>
+      <c r="E84" s="28"/>
+      <c r="F84" s="28"/>
+      <c r="G84" s="21"/>
+    </row>
+    <row r="85" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B85" s="21"/>
+      <c r="C85" s="28"/>
+      <c r="D85" s="28"/>
+      <c r="E85" s="28"/>
+      <c r="F85" s="28"/>
+      <c r="G85" s="21"/>
+    </row>
+    <row r="86" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B86" s="21"/>
+      <c r="C86" s="28"/>
+      <c r="D86" s="28"/>
+      <c r="E86" s="28"/>
+      <c r="F86" s="28"/>
+      <c r="G86" s="21"/>
+    </row>
+    <row r="87" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B87" s="21"/>
+      <c r="C87" s="28"/>
+      <c r="D87" s="28"/>
+      <c r="E87" s="28"/>
+      <c r="F87" s="28"/>
+      <c r="G87" s="21"/>
+    </row>
+    <row r="88" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B88" s="21"/>
+      <c r="C88" s="28"/>
+      <c r="D88" s="28"/>
+      <c r="E88" s="28"/>
+      <c r="F88" s="28"/>
+      <c r="G88" s="21"/>
+    </row>
+    <row r="89" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B89" s="21"/>
+      <c r="C89" s="28"/>
+      <c r="D89" s="28"/>
+      <c r="E89" s="28"/>
+      <c r="F89" s="28"/>
+      <c r="G89" s="21"/>
+    </row>
+    <row r="90" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B90" s="21"/>
+      <c r="C90" s="28"/>
+      <c r="D90" s="28"/>
+      <c r="E90" s="28"/>
+      <c r="F90" s="28"/>
+      <c r="G90" s="21"/>
+    </row>
+    <row r="91" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B91" s="21"/>
+      <c r="C91" s="28"/>
+      <c r="D91" s="28"/>
+      <c r="E91" s="28"/>
+      <c r="F91" s="28"/>
+      <c r="G91" s="21"/>
+    </row>
+    <row r="92" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B92" s="21"/>
+      <c r="C92" s="28"/>
+      <c r="D92" s="28"/>
+      <c r="E92" s="28"/>
+      <c r="F92" s="28"/>
+      <c r="G92" s="21"/>
+    </row>
+    <row r="93" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B93" s="21"/>
+      <c r="C93" s="28"/>
+      <c r="D93" s="28"/>
+      <c r="E93" s="28"/>
+      <c r="F93" s="28"/>
+      <c r="G93" s="21"/>
+    </row>
+    <row r="94" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B94" s="21"/>
+      <c r="C94" s="28"/>
+      <c r="D94" s="28"/>
+      <c r="E94" s="28"/>
+      <c r="F94" s="28"/>
+      <c r="G94" s="21"/>
+    </row>
+    <row r="95" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B95" s="21"/>
+      <c r="C95" s="28"/>
+      <c r="D95" s="28"/>
+      <c r="E95" s="28"/>
+      <c r="F95" s="28"/>
+      <c r="G95" s="21"/>
+    </row>
+    <row r="96" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B96" s="21"/>
+      <c r="C96" s="28"/>
+      <c r="D96" s="28"/>
+      <c r="E96" s="28"/>
+      <c r="F96" s="28"/>
+      <c r="G96" s="21"/>
+    </row>
+    <row r="97" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B97" s="21"/>
+      <c r="C97" s="28"/>
+      <c r="D97" s="28"/>
+      <c r="E97" s="28"/>
+      <c r="F97" s="28"/>
+      <c r="G97" s="21"/>
+    </row>
+    <row r="98" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B98" s="21"/>
+      <c r="C98" s="28"/>
+      <c r="D98" s="28"/>
+      <c r="E98" s="28"/>
+      <c r="F98" s="28"/>
+      <c r="G98" s="21"/>
+    </row>
+    <row r="99" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B99" s="21"/>
+      <c r="C99" s="28"/>
+      <c r="D99" s="28"/>
+      <c r="E99" s="28"/>
+      <c r="F99" s="28"/>
+      <c r="G99" s="21"/>
+    </row>
+    <row r="102" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B102" s="48" t="s">
+        <v>131</v>
+      </c>
+      <c r="C102" s="48"/>
+      <c r="D102" s="48"/>
+    </row>
+    <row r="103" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B103" s="49" t="s">
+        <v>133</v>
+      </c>
+      <c r="C103" s="49"/>
+      <c r="D103" s="49"/>
+    </row>
+    <row r="106" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B106" s="51" t="s">
+        <v>130</v>
+      </c>
+      <c r="C106" s="52"/>
+      <c r="D106" s="52"/>
+      <c r="E106" s="52"/>
+      <c r="F106" s="52"/>
+    </row>
+    <row r="107" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B107" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D107" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="E107" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="F107" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B108" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C108" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D108" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="E108" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="F108" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B109" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="C109" s="6">
+        <v>2000</v>
+      </c>
+      <c r="D109" s="6">
+        <v>3</v>
+      </c>
+      <c r="E109" s="6">
+        <v>4</v>
+      </c>
+      <c r="F109" s="11" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="110" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B110" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="C110" s="6">
+        <v>2000</v>
+      </c>
+      <c r="D110" s="6">
+        <v>2</v>
+      </c>
+      <c r="E110" s="6">
+        <v>1</v>
+      </c>
+      <c r="F110" s="11" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="111" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B111" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="C111" s="6">
+        <v>1</v>
+      </c>
+      <c r="D111" s="6">
+        <v>1</v>
+      </c>
+      <c r="E111" s="6">
+        <v>1</v>
+      </c>
+      <c r="F111" s="11" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="112" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B112" s="30">
+        <v>44720</v>
+      </c>
+      <c r="C112" s="6"/>
+      <c r="D112" s="6">
+        <v>1</v>
+      </c>
+      <c r="E112" s="6">
+        <v>1</v>
+      </c>
+      <c r="F112" s="11"/>
+    </row>
+    <row r="113" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="B113" s="31">
+        <v>44720</v>
+      </c>
+      <c r="C113" s="6">
+        <v>1</v>
+      </c>
+      <c r="D113" s="6">
+        <v>1</v>
+      </c>
+      <c r="E113" s="6"/>
+      <c r="F113" s="11"/>
+    </row>
+    <row r="114" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="B114" s="32">
+        <v>44721</v>
+      </c>
+      <c r="C114" s="6">
+        <v>1</v>
+      </c>
+      <c r="D114" s="6"/>
+      <c r="E114" s="6">
+        <v>1</v>
+      </c>
+      <c r="F114" s="11"/>
+    </row>
+    <row r="115" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="B115" s="32"/>
+      <c r="C115" s="6">
+        <v>3</v>
+      </c>
+      <c r="D115" s="6">
+        <v>1</v>
+      </c>
+      <c r="E115" s="6">
+        <v>2</v>
+      </c>
+      <c r="F115" s="11"/>
+    </row>
+    <row r="116" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="B116" s="33">
+        <v>44728</v>
+      </c>
+      <c r="C116" s="6">
+        <v>0</v>
+      </c>
+      <c r="D116" s="6">
+        <v>1</v>
+      </c>
+      <c r="E116" s="6">
+        <v>1</v>
+      </c>
+      <c r="F116" s="11"/>
+    </row>
+    <row r="117" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="B117" s="34">
+        <v>44729</v>
+      </c>
+      <c r="C117" s="6">
+        <v>2001</v>
+      </c>
+      <c r="D117" s="6">
+        <v>0</v>
+      </c>
+      <c r="E117" s="6">
+        <v>10</v>
+      </c>
+      <c r="F117" s="11"/>
+    </row>
+    <row r="118" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="B118" s="35">
+        <v>44727</v>
+      </c>
+      <c r="C118" s="6">
+        <v>2001</v>
+      </c>
+      <c r="D118" s="6">
+        <v>13</v>
+      </c>
+      <c r="E118" s="6">
+        <v>10</v>
+      </c>
+      <c r="F118" s="11"/>
+    </row>
+    <row r="119" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="B119" s="36">
+        <v>44729</v>
+      </c>
+      <c r="C119" s="6">
+        <v>2001</v>
+      </c>
+      <c r="D119" s="6">
+        <v>12</v>
+      </c>
+      <c r="E119" s="6">
+        <v>0</v>
+      </c>
+      <c r="F119" s="11"/>
+    </row>
+    <row r="120" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="B120" s="37">
+        <v>44722</v>
+      </c>
+      <c r="C120" s="6">
+        <v>2001</v>
+      </c>
+      <c r="D120" s="6">
+        <v>4</v>
+      </c>
+      <c r="E120" s="6">
+        <v>31</v>
+      </c>
+      <c r="F120" s="11"/>
+    </row>
+    <row r="121" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="B121" s="38">
+        <v>44720</v>
+      </c>
+      <c r="C121" s="6">
+        <v>-1</v>
+      </c>
+      <c r="D121" s="6">
+        <v>1</v>
+      </c>
+      <c r="E121" s="6">
+        <v>1</v>
+      </c>
+      <c r="F121" s="11"/>
+    </row>
+    <row r="122" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="B122" s="39">
+        <v>44729</v>
+      </c>
+      <c r="C122" s="6">
+        <v>1</v>
+      </c>
+      <c r="D122" s="6">
+        <v>-1</v>
+      </c>
+      <c r="E122" s="6">
+        <v>1</v>
+      </c>
+      <c r="F122" s="11"/>
+    </row>
+    <row r="123" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="B123" s="40">
+        <v>44728</v>
+      </c>
+      <c r="C123" s="6">
+        <v>1</v>
+      </c>
+      <c r="D123" s="6">
+        <v>1</v>
+      </c>
+      <c r="E123" s="6">
+        <v>-1</v>
+      </c>
+      <c r="F123" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="B102:D102"/>
+    <mergeCell ref="B103:D103"/>
+    <mergeCell ref="B106:F106"/>
+    <mergeCell ref="B65:G65"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="B61:D61"/>
+    <mergeCell ref="B62:D62"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B31:E31"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7ED34E8-D060-402C-99E7-2BC0710CBE80}">
+  <dimension ref="B4:E24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="2" max="2" width="28.1640625" customWidth="1"/>
+    <col min="3" max="3" width="26" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B4" s="48" t="s">
+        <v>137</v>
+      </c>
+      <c r="C4" s="48"/>
+      <c r="D4" s="48"/>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B5" s="49" t="s">
+        <v>134</v>
+      </c>
+      <c r="C5" s="49"/>
+      <c r="D5" s="49"/>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B7" s="51" t="s">
+        <v>138</v>
+      </c>
+      <c r="C7" s="52"/>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B9" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B10" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B11" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B12" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B13" s="11"/>
+      <c r="C13" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="E13" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B16" s="48" t="s">
+        <v>161</v>
+      </c>
+      <c r="C16" s="48"/>
+      <c r="D16" s="48"/>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B17" s="49" t="s">
+        <v>162</v>
+      </c>
+      <c r="C17" s="49"/>
+      <c r="D17" s="49"/>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B19" s="51" t="s">
+        <v>138</v>
+      </c>
+      <c r="C19" s="52"/>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B20" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B21" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B22" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B23" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B24" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>136</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B17:D17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
EPBDS-14306 Support yyyy-MM-dd ISO8601 date format in toDate() function
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/Dates.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/Dates.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="201">
   <si>
     <t xml:space="preserve">Method String toStringMethod (Date date)</t>
   </si>
@@ -546,6 +546,87 @@
   </si>
   <si>
     <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t>wrong input</t>
+  </si>
+  <si>
+    <t>as</t>
+  </si>
+  <si>
+    <t>wrong date</t>
+  </si>
+  <si>
+    <t>13/13/2018</t>
+  </si>
+  <si>
+    <t>null to null</t>
+  </si>
+  <si>
+    <t>01/01/0001</t>
+  </si>
+  <si>
+    <t>1/1/0001 00:00:11</t>
+  </si>
+  <si>
+    <t>05/14/1789</t>
+  </si>
+  <si>
+    <t>5/14/1789 3:30:10</t>
+  </si>
+  <si>
+    <t>12/30/2015</t>
+  </si>
+  <si>
+    <t>12/30/2015 14:42:30</t>
+  </si>
+  <si>
+    <t>05/14/3892</t>
+  </si>
+  <si>
+    <t>5/14/3892</t>
+  </si>
+  <si>
+    <t>01/01/0010</t>
+  </si>
+  <si>
+    <t>1/1/0010</t>
+  </si>
+  <si>
+    <t>01/01/2001</t>
+  </si>
+  <si>
+    <t>1/1/01</t>
+  </si>
+  <si>
+    <t>01/01/1900</t>
+  </si>
+  <si>
+    <t>12/31/1899</t>
+  </si>
+  <si>
+    <t>12/30/5555555</t>
+  </si>
+  <si>
+    <t>1/1/11</t>
+  </si>
+  <si>
+    <t>1/1/1</t>
+  </si>
+  <si>
+    <t>1980-07-12</t>
+  </si>
+  <si>
+    <t>2024-02-29</t>
+  </si>
+  <si>
+    <t>29/02/2029</t>
+  </si>
+  <si>
+    <t>29/02/2024</t>
+  </si>
+  <si>
+    <t>02/29/2024</t>
   </si>
 </sst>
 </file>
@@ -689,32 +770,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+  <cellStyleXfs count="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true" xfId="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="43">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -827,14 +889,69 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false" applyNumberFormat="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false" applyNumberFormat="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false" applyNumberFormat="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false" applyNumberFormat="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -852,9 +969,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="18.33"/>
+    <col min="2" max="2" customWidth="true" hidden="false" style="0" width="19.5" collapsed="false" outlineLevel="0"/>
+    <col min="3" max="3" customWidth="true" hidden="false" style="0" width="26.83" collapsed="false" outlineLevel="0"/>
+    <col min="4" max="5" customWidth="true" hidden="false" style="0" width="18.33" collapsed="false" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1472,9 +1589,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="18.33"/>
+    <col min="2" max="2" customWidth="true" hidden="false" style="0" width="19.5" collapsed="false" outlineLevel="0"/>
+    <col min="3" max="3" customWidth="true" hidden="false" style="0" width="26.83" collapsed="false" outlineLevel="0"/>
+    <col min="4" max="5" customWidth="true" hidden="false" style="0" width="18.33" collapsed="false" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1524,128 +1641,154 @@
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>21</v>
-      </c>
+        <v>196</v>
+      </c>
+      <c r="C9" s="40" t="n">
+        <v>29414.0</v>
+      </c>
+      <c r="D9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="C10" s="10" t="n">
-        <v>40544</v>
-      </c>
+        <v>197</v>
+      </c>
+      <c r="C10" s="40" t="s">
+        <v>197</v>
+      </c>
+      <c r="D10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>10</v>
-      </c>
+        <v>200</v>
+      </c>
+      <c r="C11" s="40" t="s">
+        <v>197</v>
+      </c>
+      <c r="D11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="8" t="s">
-        <v>8</v>
+        <v>195</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>8</v>
-      </c>
+        <v>179</v>
+      </c>
+      <c r="D12" s="39"/>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>9</v>
-      </c>
+        <v>194</v>
+      </c>
+      <c r="C13" s="10" t="n">
+        <v>40544.0</v>
+      </c>
+      <c r="D13" s="37"/>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="8" t="s">
-        <v>11</v>
+        <v>193</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>7</v>
-      </c>
+        <v>193</v>
+      </c>
+      <c r="D14" s="36"/>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="8" t="s">
-        <v>12</v>
+        <v>192</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>13</v>
-      </c>
+        <v>192</v>
+      </c>
+      <c r="D15" s="35"/>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="8" t="s">
-        <v>14</v>
+        <v>191</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>15</v>
-      </c>
+        <v>191</v>
+      </c>
+      <c r="D16" s="34"/>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="8" t="s">
-        <v>16</v>
+        <v>190</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>17</v>
-      </c>
+        <v>189</v>
+      </c>
+      <c r="D17" s="33"/>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="8" t="s">
-        <v>18</v>
+        <v>188</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>19</v>
-      </c>
+        <v>187</v>
+      </c>
+      <c r="D18" s="32"/>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="8" t="s">
-        <v>20</v>
+        <v>186</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>21</v>
-      </c>
+        <v>185</v>
+      </c>
+      <c r="D19" s="31"/>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="11"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="0" t="s">
-        <v>78</v>
-      </c>
+      <c r="B20" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="D20" s="30"/>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="C21" s="11"/>
-      <c r="D21" s="0" t="s">
-        <v>80</v>
-      </c>
+      <c r="B21" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="D21" s="29"/>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="C22" s="11"/>
-      <c r="D22" s="0" t="s">
-        <v>82</v>
-      </c>
+      <c r="B22" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="D22" s="28"/>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="20"/>
-      <c r="C23" s="21"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="0" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="20"/>
-      <c r="C24" s="21"/>
+      <c r="B24" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="C24" s="11"/>
+      <c r="D24" s="0" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="20"/>
-      <c r="C25" s="21"/>
+      <c r="B25" t="s" s="11">
+        <v>175</v>
+      </c>
+      <c r="C25" s="11"/>
+      <c r="D25" t="s" s="0">
+        <v>174</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="20"/>
@@ -2135,13 +2278,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="23.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="43.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="27.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="24.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="41.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="31.83"/>
+    <col min="2" max="3" customWidth="true" hidden="false" style="0" width="23.35" collapsed="false" outlineLevel="0"/>
+    <col min="4" max="4" customWidth="true" hidden="false" style="0" width="43.51" collapsed="false" outlineLevel="0"/>
+    <col min="5" max="5" customWidth="true" hidden="false" style="0" width="27.99" collapsed="false" outlineLevel="0"/>
+    <col min="6" max="6" customWidth="true" hidden="false" style="0" width="11.5" collapsed="false" outlineLevel="0"/>
+    <col min="7" max="7" customWidth="true" hidden="false" style="0" width="24.49" collapsed="false" outlineLevel="0"/>
+    <col min="8" max="8" customWidth="true" hidden="false" style="0" width="41.49" collapsed="false" outlineLevel="0"/>
+    <col min="9" max="9" customWidth="true" hidden="false" style="0" width="31.83" collapsed="false" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4028,12 +4171,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="40.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="23.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="28.84"/>
+    <col min="2" max="2" customWidth="true" hidden="false" style="0" width="23.35" collapsed="false" outlineLevel="0"/>
+    <col min="3" max="3" customWidth="true" hidden="false" style="0" width="19.65" collapsed="false" outlineLevel="0"/>
+    <col min="4" max="4" customWidth="true" hidden="false" style="0" width="40.15" collapsed="false" outlineLevel="0"/>
+    <col min="5" max="5" customWidth="true" hidden="false" style="0" width="19.84" collapsed="false" outlineLevel="0"/>
+    <col min="6" max="6" customWidth="true" hidden="false" style="0" width="23.83" collapsed="false" outlineLevel="0"/>
+    <col min="7" max="7" customWidth="true" hidden="false" style="0" width="28.84" collapsed="false" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5289,8 +5432,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26"/>
+    <col min="2" max="2" customWidth="true" hidden="false" style="0" width="28.16" collapsed="false" outlineLevel="0"/>
+    <col min="3" max="3" customWidth="true" hidden="false" style="0" width="26.0" collapsed="false" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>